<commit_message>
updates CA avant migration
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF006510-9E74-2744-90E9-FBA206921C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3955151E-573B-4743-B084-4F51E6EEF510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
@@ -1624,7 +1624,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1968,6 +1968,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers" xfId="2" builtinId="3"/>
@@ -4236,99 +4237,99 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>207</v>
+        <v>108</v>
       </c>
       <c r="B38" s="102"/>
       <c r="C38" s="92" t="s">
-        <v>277</v>
+        <v>98</v>
       </c>
       <c r="D38" s="92"/>
       <c r="E38" s="56"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B39" s="102"/>
       <c r="C39" s="92" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D39" s="92"/>
       <c r="E39" s="56"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" s="102"/>
+        <v>208</v>
+      </c>
+      <c r="B40" s="119"/>
       <c r="C40" s="92" t="s">
-        <v>96</v>
+        <v>278</v>
       </c>
       <c r="D40" s="92"/>
       <c r="E40" s="56"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>208</v>
-      </c>
-      <c r="B41" s="97"/>
+        <v>209</v>
+      </c>
+      <c r="B41" s="119"/>
       <c r="C41" s="92" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D41" s="92"/>
       <c r="E41" s="56"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>209</v>
-      </c>
-      <c r="B42" s="97"/>
+        <v>210</v>
+      </c>
+      <c r="B42" s="119"/>
       <c r="C42" s="92" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D42" s="92"/>
       <c r="E42" s="56"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>210</v>
-      </c>
-      <c r="B43" s="97"/>
+        <v>211</v>
+      </c>
+      <c r="B43" s="119"/>
       <c r="C43" s="92" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D43" s="92"/>
       <c r="E43" s="56"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>211</v>
-      </c>
-      <c r="B44" s="97"/>
+        <v>212</v>
+      </c>
+      <c r="B44" s="119"/>
       <c r="C44" s="92" t="s">
-        <v>281</v>
+        <v>103</v>
       </c>
       <c r="D44" s="92"/>
       <c r="E44" s="56"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>212</v>
-      </c>
-      <c r="B45" s="97"/>
+        <v>213</v>
+      </c>
+      <c r="B45" s="119"/>
       <c r="C45" s="92" t="s">
-        <v>103</v>
+        <v>269</v>
       </c>
       <c r="D45" s="92"/>
       <c r="E45" s="56"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>213</v>
-      </c>
-      <c r="B46" s="97"/>
+        <v>207</v>
+      </c>
+      <c r="B46" s="119"/>
       <c r="C46" s="92" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="D46" s="92"/>
       <c r="E46" s="56"/>
@@ -4856,101 +4857,101 @@
       <c r="D87" s="92"/>
       <c r="E87" s="56"/>
     </row>
-    <row r="88" spans="1:5" ht="30">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B88" s="96"/>
       <c r="C88" s="92" t="s">
-        <v>308</v>
+        <v>137</v>
       </c>
       <c r="D88" s="92"/>
       <c r="E88" s="56"/>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>234</v>
-      </c>
-      <c r="B89" s="96"/>
+        <v>235</v>
+      </c>
+      <c r="B89" s="119"/>
       <c r="C89" s="92" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D89" s="92"/>
       <c r="E89" s="56"/>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>235</v>
-      </c>
-      <c r="B90" s="97"/>
+        <v>236</v>
+      </c>
+      <c r="B90" s="119"/>
       <c r="C90" s="92" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D90" s="92"/>
       <c r="E90" s="56"/>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>236</v>
-      </c>
-      <c r="B91" s="97"/>
+        <v>237</v>
+      </c>
+      <c r="B91" s="119"/>
       <c r="C91" s="92" t="s">
-        <v>141</v>
+        <v>309</v>
       </c>
       <c r="D91" s="92"/>
       <c r="E91" s="56"/>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>237</v>
-      </c>
-      <c r="B92" s="97"/>
+        <v>238</v>
+      </c>
+      <c r="B92" s="119"/>
       <c r="C92" s="92" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D92" s="92"/>
       <c r="E92" s="56"/>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>238</v>
-      </c>
-      <c r="B93" s="97"/>
+        <v>239</v>
+      </c>
+      <c r="B93" s="119"/>
       <c r="C93" s="92" t="s">
-        <v>310</v>
+        <v>140</v>
       </c>
       <c r="D93" s="92"/>
       <c r="E93" s="56"/>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>239</v>
-      </c>
-      <c r="B94" s="97"/>
+        <v>240</v>
+      </c>
+      <c r="B94" s="119"/>
       <c r="C94" s="92" t="s">
-        <v>140</v>
+        <v>311</v>
       </c>
       <c r="D94" s="92"/>
       <c r="E94" s="56"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" ht="30">
       <c r="A95" t="s">
-        <v>240</v>
-      </c>
-      <c r="B95" s="97"/>
+        <v>241</v>
+      </c>
+      <c r="B95" s="119"/>
       <c r="C95" s="92" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D95" s="92"/>
       <c r="E95" s="56"/>
     </row>
     <row r="96" spans="1:5" ht="30">
       <c r="A96" t="s">
-        <v>241</v>
-      </c>
-      <c r="B96" s="97"/>
+        <v>233</v>
+      </c>
+      <c r="B96" s="119"/>
       <c r="C96" s="92" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D96" s="92"/>
       <c r="E96" s="56"/>
@@ -4971,24 +4972,24 @@
     </row>
     <row r="98" spans="1:5" ht="16" thickTop="1"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bE8pqAMZHmApP/xMh9/Go5Qo7PIR2/h4mvCS1ky4exo5CQYvtDWAyyAH4H1KuuvSadlyCPrBK3YhseJt2XLjXQ==" saltValue="XqjIwYf6cm+iXTYNNCzffA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="R0NN/OwuLECm17r344GUX0QWIHifkUxZcGRVPuxNXCBVjVU4w2aEkxSCqEstdN7RNRk9MurHyRVgNaeeCYmYcQ==" saltValue="ZzwqWq5f3y3A+QaIQ+gb5g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="15">
+    <mergeCell ref="B87:B96"/>
     <mergeCell ref="B78:B80"/>
     <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B87:B96"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="B14:B22"/>
     <mergeCell ref="B24:B28"/>
     <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B37:B46"/>
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="B56:B61"/>
     <mergeCell ref="B63:B71"/>
     <mergeCell ref="B73:B76"/>
+    <mergeCell ref="B37:B46"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A12">
     <cfRule type="expression" dxfId="1" priority="3">

</xml_diff>

<commit_message>
maj fiche agent ca pp
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AF512B-FC23-2946-BE80-696F8298C01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966DCB2E-8B95-3548-A00F-6C32B028A003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="S0xIUhd+qm/mil3mjEDLzBXqSnUj+E9UJlwfUt2w9pzFPXpGrV21CR6+VbcA2GUl+o5ORpHAcx1Tl5P1yPCQ/w==" workbookSaltValue="Ic6K1fVcoeoWgJU+jzPQ6w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille de temps" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="356">
   <si>
     <t>Temps de travail d'un magistrat</t>
   </si>
@@ -1340,6 +1340,9 @@
   </si>
   <si>
     <t>13.</t>
+  </si>
+  <si>
+    <t>TOTAL PP</t>
   </si>
 </sst>
 </file>
@@ -2128,6 +2131,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2142,9 +2155,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2199,13 +2209,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2213,7 +2216,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2288,128 +2291,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="7" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="7" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4363,12 +4244,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="121"/>
-      <c r="B6" s="142" t="s">
+      <c r="B6" s="146" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="142"/>
-      <c r="D6" s="142"/>
-      <c r="E6" s="143"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
+      <c r="E6" s="147"/>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
@@ -4393,8 +4274,8 @@
       <c r="B8" s="130" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="144"/>
-      <c r="D8" s="145"/>
+      <c r="C8" s="148"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="131" t="s">
         <v>90</v>
       </c>
@@ -4404,7 +4285,7 @@
       <c r="A9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="142" t="s">
         <v>92</v>
       </c>
       <c r="C9" s="132" t="s">
@@ -4418,7 +4299,7 @@
       <c r="A10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="146"/>
+      <c r="B10" s="144"/>
       <c r="C10" s="132" t="s">
         <v>249</v>
       </c>
@@ -4430,7 +4311,7 @@
       <c r="A11" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="146"/>
+      <c r="B11" s="144"/>
       <c r="C11" s="132" t="s">
         <v>250</v>
       </c>
@@ -4442,7 +4323,7 @@
       <c r="A12" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="146"/>
+      <c r="B12" s="144"/>
       <c r="C12" s="132" t="s">
         <v>96</v>
       </c>
@@ -4473,7 +4354,7 @@
       <c r="A14" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="142" t="s">
         <v>252</v>
       </c>
       <c r="C14" s="132" t="s">
@@ -4487,7 +4368,7 @@
       <c r="A15" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="146"/>
+      <c r="B15" s="144"/>
       <c r="C15" s="132" t="s">
         <v>254</v>
       </c>
@@ -4499,7 +4380,7 @@
       <c r="A16" t="s">
         <v>101</v>
       </c>
-      <c r="B16" s="146"/>
+      <c r="B16" s="144"/>
       <c r="C16" s="132" t="s">
         <v>128</v>
       </c>
@@ -4511,7 +4392,7 @@
       <c r="A17" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="146"/>
+      <c r="B17" s="144"/>
       <c r="C17" s="132" t="s">
         <v>255</v>
       </c>
@@ -4523,7 +4404,7 @@
       <c r="A18" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="166"/>
+      <c r="B18" s="145"/>
       <c r="C18" s="132" t="s">
         <v>256</v>
       </c>
@@ -4535,7 +4416,7 @@
       <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="166"/>
+      <c r="B19" s="145"/>
       <c r="C19" s="132" t="s">
         <v>257</v>
       </c>
@@ -4547,7 +4428,7 @@
       <c r="A20" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="166"/>
+      <c r="B20" s="145"/>
       <c r="C20" s="132" t="s">
         <v>258</v>
       </c>
@@ -4559,7 +4440,7 @@
       <c r="A21" t="s">
         <v>107</v>
       </c>
-      <c r="B21" s="166"/>
+      <c r="B21" s="145"/>
       <c r="C21" s="132" t="s">
         <v>259</v>
       </c>
@@ -4571,7 +4452,7 @@
       <c r="A22" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="166"/>
+      <c r="B22" s="145"/>
       <c r="C22" s="132" t="s">
         <v>260</v>
       </c>
@@ -4602,7 +4483,7 @@
       <c r="A24" t="s">
         <v>262</v>
       </c>
-      <c r="B24" s="165" t="s">
+      <c r="B24" s="142" t="s">
         <v>263</v>
       </c>
       <c r="C24" s="132" t="s">
@@ -4616,7 +4497,7 @@
       <c r="A25" t="s">
         <v>110</v>
       </c>
-      <c r="B25" s="146"/>
+      <c r="B25" s="144"/>
       <c r="C25" s="132" t="s">
         <v>265</v>
       </c>
@@ -4628,7 +4509,7 @@
       <c r="A26" t="s">
         <v>112</v>
       </c>
-      <c r="B26" s="146"/>
+      <c r="B26" s="144"/>
       <c r="C26" s="132" t="s">
         <v>266</v>
       </c>
@@ -4640,7 +4521,7 @@
       <c r="A27" t="s">
         <v>267</v>
       </c>
-      <c r="B27" s="146"/>
+      <c r="B27" s="144"/>
       <c r="C27" s="132" t="s">
         <v>106</v>
       </c>
@@ -4652,7 +4533,7 @@
       <c r="A28" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="166"/>
+      <c r="B28" s="145"/>
       <c r="C28" s="132" t="s">
         <v>268</v>
       </c>
@@ -4683,7 +4564,7 @@
       <c r="A30" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="165" t="s">
+      <c r="B30" s="142" t="s">
         <v>270</v>
       </c>
       <c r="C30" s="132" t="s">
@@ -4697,7 +4578,7 @@
       <c r="A31" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="146"/>
+      <c r="B31" s="144"/>
       <c r="C31" s="132" t="s">
         <v>113</v>
       </c>
@@ -4709,7 +4590,7 @@
       <c r="A32" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="146"/>
+      <c r="B32" s="144"/>
       <c r="C32" s="132" t="s">
         <v>271</v>
       </c>
@@ -4721,7 +4602,7 @@
       <c r="A33" t="s">
         <v>122</v>
       </c>
-      <c r="B33" s="146"/>
+      <c r="B33" s="144"/>
       <c r="C33" s="132" t="s">
         <v>114</v>
       </c>
@@ -4733,7 +4614,7 @@
       <c r="A34" t="s">
         <v>124</v>
       </c>
-      <c r="B34" s="166"/>
+      <c r="B34" s="145"/>
       <c r="C34" s="132" t="s">
         <v>272</v>
       </c>
@@ -4745,7 +4626,7 @@
       <c r="A35" t="s">
         <v>126</v>
       </c>
-      <c r="B35" s="166"/>
+      <c r="B35" s="145"/>
       <c r="C35" s="132" t="s">
         <v>116</v>
       </c>
@@ -4776,7 +4657,7 @@
       <c r="A37" t="s">
         <v>133</v>
       </c>
-      <c r="B37" s="165" t="s">
+      <c r="B37" s="142" t="s">
         <v>118</v>
       </c>
       <c r="C37" s="132" t="s">
@@ -4790,7 +4671,7 @@
       <c r="A38" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="146"/>
+      <c r="B38" s="144"/>
       <c r="C38" s="132" t="s">
         <v>125</v>
       </c>
@@ -4802,7 +4683,7 @@
       <c r="A39" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="146"/>
+      <c r="B39" s="144"/>
       <c r="C39" s="132" t="s">
         <v>123</v>
       </c>
@@ -4814,7 +4695,7 @@
       <c r="A40" t="s">
         <v>274</v>
       </c>
-      <c r="B40" s="166"/>
+      <c r="B40" s="145"/>
       <c r="C40" s="132" t="s">
         <v>275</v>
       </c>
@@ -4826,7 +4707,7 @@
       <c r="A41" t="s">
         <v>276</v>
       </c>
-      <c r="B41" s="166"/>
+      <c r="B41" s="145"/>
       <c r="C41" s="132" t="s">
         <v>277</v>
       </c>
@@ -4838,7 +4719,7 @@
       <c r="A42" t="s">
         <v>278</v>
       </c>
-      <c r="B42" s="166"/>
+      <c r="B42" s="145"/>
       <c r="C42" s="132" t="s">
         <v>279</v>
       </c>
@@ -4850,7 +4731,7 @@
       <c r="A43" t="s">
         <v>280</v>
       </c>
-      <c r="B43" s="166"/>
+      <c r="B43" s="145"/>
       <c r="C43" s="132" t="s">
         <v>281</v>
       </c>
@@ -4862,7 +4743,7 @@
       <c r="A44" t="s">
         <v>282</v>
       </c>
-      <c r="B44" s="166"/>
+      <c r="B44" s="145"/>
       <c r="C44" s="132" t="s">
         <v>130</v>
       </c>
@@ -4874,7 +4755,7 @@
       <c r="A45" t="s">
         <v>283</v>
       </c>
-      <c r="B45" s="166"/>
+      <c r="B45" s="145"/>
       <c r="C45" s="132" t="s">
         <v>259</v>
       </c>
@@ -4886,7 +4767,7 @@
       <c r="A46" t="s">
         <v>284</v>
       </c>
-      <c r="B46" s="166"/>
+      <c r="B46" s="145"/>
       <c r="C46" s="132" t="s">
         <v>285</v>
       </c>
@@ -4917,7 +4798,7 @@
       <c r="A48" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="165" t="s">
+      <c r="B48" s="142" t="s">
         <v>134</v>
       </c>
       <c r="C48" s="132" t="s">
@@ -4931,7 +4812,7 @@
       <c r="A49" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="146"/>
+      <c r="B49" s="144"/>
       <c r="C49" s="132" t="s">
         <v>287</v>
       </c>
@@ -4943,7 +4824,7 @@
       <c r="A50" t="s">
         <v>288</v>
       </c>
-      <c r="B50" s="146"/>
+      <c r="B50" s="144"/>
       <c r="C50" s="132" t="s">
         <v>289</v>
       </c>
@@ -4955,7 +4836,7 @@
       <c r="A51" t="s">
         <v>290</v>
       </c>
-      <c r="B51" s="146"/>
+      <c r="B51" s="144"/>
       <c r="C51" s="132" t="s">
         <v>137</v>
       </c>
@@ -4986,7 +4867,7 @@
       <c r="A53" t="s">
         <v>145</v>
       </c>
-      <c r="B53" s="165" t="s">
+      <c r="B53" s="142" t="s">
         <v>291</v>
       </c>
       <c r="C53" s="132" t="s">
@@ -5000,7 +4881,7 @@
       <c r="A54" t="s">
         <v>146</v>
       </c>
-      <c r="B54" s="167"/>
+      <c r="B54" s="143"/>
       <c r="C54" s="132" t="s">
         <v>143</v>
       </c>
@@ -5031,7 +4912,7 @@
       <c r="A56" t="s">
         <v>148</v>
       </c>
-      <c r="B56" s="165" t="s">
+      <c r="B56" s="142" t="s">
         <v>293</v>
       </c>
       <c r="C56" s="132" t="s">
@@ -5045,7 +4926,7 @@
       <c r="A57" t="s">
         <v>149</v>
       </c>
-      <c r="B57" s="146"/>
+      <c r="B57" s="144"/>
       <c r="C57" s="132" t="s">
         <v>295</v>
       </c>
@@ -5057,7 +4938,7 @@
       <c r="A58" t="s">
         <v>150</v>
       </c>
-      <c r="B58" s="146"/>
+      <c r="B58" s="144"/>
       <c r="C58" s="132" t="s">
         <v>296</v>
       </c>
@@ -5069,7 +4950,7 @@
       <c r="A59" t="s">
         <v>151</v>
       </c>
-      <c r="B59" s="146"/>
+      <c r="B59" s="144"/>
       <c r="C59" s="132" t="s">
         <v>297</v>
       </c>
@@ -5081,7 +4962,7 @@
       <c r="A60" t="s">
         <v>298</v>
       </c>
-      <c r="B60" s="166"/>
+      <c r="B60" s="145"/>
       <c r="C60" s="132" t="s">
         <v>299</v>
       </c>
@@ -5093,7 +4974,7 @@
       <c r="A61" t="s">
         <v>300</v>
       </c>
-      <c r="B61" s="166"/>
+      <c r="B61" s="145"/>
       <c r="C61" s="132" t="s">
         <v>129</v>
       </c>
@@ -5124,7 +5005,7 @@
       <c r="A63" t="s">
         <v>153</v>
       </c>
-      <c r="B63" s="165" t="s">
+      <c r="B63" s="142" t="s">
         <v>302</v>
       </c>
       <c r="C63" s="132" t="s">
@@ -5138,7 +5019,7 @@
       <c r="A64" t="s">
         <v>154</v>
       </c>
-      <c r="B64" s="146"/>
+      <c r="B64" s="144"/>
       <c r="C64" s="132" t="s">
         <v>303</v>
       </c>
@@ -5150,7 +5031,7 @@
       <c r="A65" t="s">
         <v>155</v>
       </c>
-      <c r="B65" s="146"/>
+      <c r="B65" s="144"/>
       <c r="C65" s="132" t="s">
         <v>304</v>
       </c>
@@ -5162,7 +5043,7 @@
       <c r="A66" t="s">
         <v>156</v>
       </c>
-      <c r="B66" s="146"/>
+      <c r="B66" s="144"/>
       <c r="C66" s="132" t="s">
         <v>305</v>
       </c>
@@ -5174,7 +5055,7 @@
       <c r="A67" t="s">
         <v>306</v>
       </c>
-      <c r="B67" s="166"/>
+      <c r="B67" s="145"/>
       <c r="C67" s="132" t="s">
         <v>307</v>
       </c>
@@ -5186,7 +5067,7 @@
       <c r="A68" t="s">
         <v>308</v>
       </c>
-      <c r="B68" s="166"/>
+      <c r="B68" s="145"/>
       <c r="C68" s="132" t="s">
         <v>309</v>
       </c>
@@ -5198,7 +5079,7 @@
       <c r="A69" t="s">
         <v>310</v>
       </c>
-      <c r="B69" s="166"/>
+      <c r="B69" s="145"/>
       <c r="C69" s="132" t="s">
         <v>311</v>
       </c>
@@ -5210,7 +5091,7 @@
       <c r="A70" t="s">
         <v>312</v>
       </c>
-      <c r="B70" s="166"/>
+      <c r="B70" s="145"/>
       <c r="C70" s="132" t="s">
         <v>313</v>
       </c>
@@ -5222,7 +5103,7 @@
       <c r="A71" t="s">
         <v>314</v>
       </c>
-      <c r="B71" s="166"/>
+      <c r="B71" s="145"/>
       <c r="C71" s="132" t="s">
         <v>315</v>
       </c>
@@ -5253,7 +5134,7 @@
       <c r="A73" t="s">
         <v>158</v>
       </c>
-      <c r="B73" s="165" t="s">
+      <c r="B73" s="142" t="s">
         <v>317</v>
       </c>
       <c r="C73" s="132" t="s">
@@ -5267,7 +5148,7 @@
       <c r="A74" t="s">
         <v>159</v>
       </c>
-      <c r="B74" s="146"/>
+      <c r="B74" s="144"/>
       <c r="C74" s="132" t="s">
         <v>318</v>
       </c>
@@ -5279,7 +5160,7 @@
       <c r="A75" t="s">
         <v>319</v>
       </c>
-      <c r="B75" s="146"/>
+      <c r="B75" s="144"/>
       <c r="C75" s="132" t="s">
         <v>320</v>
       </c>
@@ -5291,7 +5172,7 @@
       <c r="A76" t="s">
         <v>321</v>
       </c>
-      <c r="B76" s="146"/>
+      <c r="B76" s="144"/>
       <c r="C76" s="132" t="s">
         <v>322</v>
       </c>
@@ -5322,7 +5203,7 @@
       <c r="A78" t="s">
         <v>161</v>
       </c>
-      <c r="B78" s="165" t="s">
+      <c r="B78" s="142" t="s">
         <v>324</v>
       </c>
       <c r="C78" s="132" t="s">
@@ -5336,7 +5217,7 @@
       <c r="A79" t="s">
         <v>326</v>
       </c>
-      <c r="B79" s="167"/>
+      <c r="B79" s="143"/>
       <c r="C79" s="132" t="s">
         <v>327</v>
       </c>
@@ -5348,7 +5229,7 @@
       <c r="A80" t="s">
         <v>165</v>
       </c>
-      <c r="B80" s="167"/>
+      <c r="B80" s="143"/>
       <c r="C80" s="132" t="s">
         <v>328</v>
       </c>
@@ -5379,7 +5260,7 @@
       <c r="A82" t="s">
         <v>330</v>
       </c>
-      <c r="B82" s="165" t="s">
+      <c r="B82" s="142" t="s">
         <v>225</v>
       </c>
       <c r="C82" s="132" t="s">
@@ -5393,7 +5274,7 @@
       <c r="A83" t="s">
         <v>332</v>
       </c>
-      <c r="B83" s="167"/>
+      <c r="B83" s="143"/>
       <c r="C83" s="132" t="s">
         <v>333</v>
       </c>
@@ -5405,7 +5286,7 @@
       <c r="A84" t="s">
         <v>334</v>
       </c>
-      <c r="B84" s="167"/>
+      <c r="B84" s="143"/>
       <c r="C84" s="132" t="s">
         <v>335</v>
       </c>
@@ -5417,7 +5298,7 @@
       <c r="A85" t="s">
         <v>336</v>
       </c>
-      <c r="B85" s="166"/>
+      <c r="B85" s="145"/>
       <c r="C85" s="132" t="s">
         <v>337</v>
       </c>
@@ -5430,7 +5311,7 @@
         <v>338</v>
       </c>
       <c r="B86" s="134" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="C86" s="135" t="s">
         <v>251</v>
@@ -5448,7 +5329,7 @@
       <c r="A87" t="s">
         <v>339</v>
       </c>
-      <c r="B87" s="165" t="s">
+      <c r="B87" s="142" t="s">
         <v>162</v>
       </c>
       <c r="C87" s="132" t="s">
@@ -5462,7 +5343,7 @@
       <c r="A88" t="s">
         <v>340</v>
       </c>
-      <c r="B88" s="167"/>
+      <c r="B88" s="143"/>
       <c r="C88" s="132" t="s">
         <v>164</v>
       </c>
@@ -5474,7 +5355,7 @@
       <c r="A89" t="s">
         <v>341</v>
       </c>
-      <c r="B89" s="166"/>
+      <c r="B89" s="145"/>
       <c r="C89" s="132" t="s">
         <v>166</v>
       </c>
@@ -5486,7 +5367,7 @@
       <c r="A90" t="s">
         <v>342</v>
       </c>
-      <c r="B90" s="166"/>
+      <c r="B90" s="145"/>
       <c r="C90" s="132" t="s">
         <v>168</v>
       </c>
@@ -5498,7 +5379,7 @@
       <c r="A91" t="s">
         <v>343</v>
       </c>
-      <c r="B91" s="166"/>
+      <c r="B91" s="145"/>
       <c r="C91" s="132" t="s">
         <v>344</v>
       </c>
@@ -5510,7 +5391,7 @@
       <c r="A92" t="s">
         <v>345</v>
       </c>
-      <c r="B92" s="166"/>
+      <c r="B92" s="145"/>
       <c r="C92" s="132" t="s">
         <v>346</v>
       </c>
@@ -5522,7 +5403,7 @@
       <c r="A93" t="s">
         <v>347</v>
       </c>
-      <c r="B93" s="166"/>
+      <c r="B93" s="145"/>
       <c r="C93" s="132" t="s">
         <v>167</v>
       </c>
@@ -5534,7 +5415,7 @@
       <c r="A94" t="s">
         <v>348</v>
       </c>
-      <c r="B94" s="166"/>
+      <c r="B94" s="145"/>
       <c r="C94" s="132" t="s">
         <v>349</v>
       </c>
@@ -5546,7 +5427,7 @@
       <c r="A95" t="s">
         <v>350</v>
       </c>
-      <c r="B95" s="166"/>
+      <c r="B95" s="145"/>
       <c r="C95" s="132" t="s">
         <v>351</v>
       </c>
@@ -5558,7 +5439,7 @@
       <c r="A96" t="s">
         <v>352</v>
       </c>
-      <c r="B96" s="166"/>
+      <c r="B96" s="145"/>
       <c r="C96" s="132" t="s">
         <v>353</v>
       </c>
@@ -5607,14 +5488,9 @@
     </row>
     <row r="104" spans="1:6" ht="98" hidden="1" customHeight="1"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8pHsP8Orr0iZLuUMM2rGFaz3ekNGAYUcVvRzu2EAREr2lc/jzP3/RYYCc4mUnLnvwEeBvW6S1oWd7F3zifwLCg==" saltValue="xY4dINKA22IA4Y6jzZnb4w==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="1b5cR/Y9gE1aCr4AZysTr2nkvHi+VUlUqFo95Xb2iAselYPtX7csV35FQfkFR4Dq/34I5Up+zbOh3kFgt3nfkA==" saltValue="dBSUhmRnhYZe8qrAXcguXA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="15">
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="B63:B71"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B78:B80"/>
     <mergeCell ref="B82:B85"/>
     <mergeCell ref="B87:B96"/>
     <mergeCell ref="B6:E6"/>
@@ -5625,6 +5501,11 @@
     <mergeCell ref="B30:B35"/>
     <mergeCell ref="B37:B46"/>
     <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="B63:B71"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="B78:B80"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A12">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -6243,10 +6124,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="27"/>
-      <c r="F4" s="152" t="s">
+      <c r="F4" s="155" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="153"/>
+      <c r="G4" s="156"/>
       <c r="H4" s="71"/>
       <c r="I4" s="2">
         <v>208</v>
@@ -6257,10 +6138,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="F5" s="154" t="s">
+      <c r="F5" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="155"/>
+      <c r="G5" s="158"/>
       <c r="H5" s="72"/>
       <c r="I5" s="6">
         <v>8</v>
@@ -6276,28 +6157,28 @@
       <c r="H6" s="35"/>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="150" t="s">
+      <c r="B7" s="153" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="149" t="s">
+      <c r="E7" s="152" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="149"/>
+      <c r="F7" s="152"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="147" t="s">
+      <c r="I7" s="150" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="69"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="151"/>
-      <c r="I8" s="148"/>
+      <c r="B8" s="154"/>
+      <c r="I8" s="151"/>
       <c r="J8" s="70"/>
       <c r="L8"/>
     </row>
@@ -6339,7 +6220,7 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="153" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="32" t="s">
@@ -6355,11 +6236,11 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="151"/>
+      <c r="B13" s="154"/>
       <c r="C13" s="77"/>
       <c r="D13" s="77"/>
       <c r="E13" s="73"/>
-      <c r="G13" s="148" t="s">
+      <c r="G13" s="151" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="70"/>
@@ -6374,7 +6255,7 @@
       <c r="E14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="148"/>
+      <c r="G14" s="151"/>
       <c r="H14" s="70"/>
       <c r="I14" s="10"/>
     </row>
@@ -6504,14 +6385,14 @@
       </c>
       <c r="C3" s="114"/>
       <c r="D3" s="26"/>
-      <c r="F3" s="156" t="s">
+      <c r="F3" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="158"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
+      <c r="K3" s="161"/>
       <c r="L3"/>
     </row>
     <row r="4" spans="2:12" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
@@ -6520,10 +6401,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="27"/>
-      <c r="F4" s="152" t="s">
+      <c r="F4" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="153"/>
+      <c r="G4" s="156"/>
       <c r="H4" s="71"/>
       <c r="I4" s="10">
         <v>1607</v>
@@ -6534,10 +6415,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="F5" s="154" t="s">
+      <c r="F5" s="157" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="155"/>
+      <c r="G5" s="158"/>
       <c r="H5" s="72"/>
       <c r="I5" s="104">
         <v>35</v>
@@ -6554,28 +6435,28 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="150" t="s">
+      <c r="B7" s="153" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="149" t="s">
+      <c r="E7" s="152" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="149"/>
+      <c r="F7" s="152"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="147" t="s">
+      <c r="I7" s="150" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="69"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="151"/>
-      <c r="I8" s="148"/>
+      <c r="B8" s="154"/>
+      <c r="I8" s="151"/>
       <c r="J8" s="70"/>
       <c r="L8"/>
     </row>
@@ -6618,7 +6499,7 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="153" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="118" t="s">
@@ -6634,11 +6515,11 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="151"/>
+      <c r="B13" s="154"/>
       <c r="C13" s="119"/>
       <c r="D13" s="77"/>
       <c r="E13" s="73"/>
-      <c r="G13" s="148" t="s">
+      <c r="G13" s="151" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="70"/>
@@ -6653,7 +6534,7 @@
       <c r="E14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="148"/>
+      <c r="G14" s="151"/>
       <c r="H14" s="70"/>
       <c r="I14" s="10"/>
     </row>
@@ -6769,30 +6650,30 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="3:9" ht="54.75" customHeight="1">
-      <c r="C2" s="160" t="s">
+      <c r="C2" s="163" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
     </row>
     <row r="3" spans="3:9" ht="27.75" customHeight="1">
       <c r="C3" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="159" t="s">
+      <c r="D3" s="162" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="159"/>
-      <c r="F3" s="161" t="s">
+      <c r="E3" s="162"/>
+      <c r="F3" s="164" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
+      <c r="G3" s="164"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="164"/>
     </row>
     <row r="4" spans="3:9" ht="23.25" customHeight="1">
       <c r="C4" s="40" t="s">
@@ -7048,26 +6929,26 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="3:12" ht="46.5" customHeight="1">
-      <c r="E2" s="162" t="s">
+      <c r="E2" s="165" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
-      <c r="K2" s="162"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
+      <c r="K2" s="165"/>
     </row>
     <row r="3" spans="3:12" ht="53.25" customHeight="1">
-      <c r="E3" s="163" t="s">
+      <c r="E3" s="166" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="163"/>
-      <c r="J3" s="163"/>
-      <c r="K3" s="163"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="3:12" ht="20.75" customHeight="1">
       <c r="E4" s="61"/>
@@ -7126,10 +7007,10 @@
       <c r="I8" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="161" t="s">
+      <c r="J8" s="164" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="161"/>
+      <c r="K8" s="164"/>
     </row>
     <row r="9" spans="3:12" ht="14" customHeight="1">
       <c r="D9" s="39"/>
@@ -7149,11 +7030,11 @@
       <c r="H10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="164" t="s">
+      <c r="I10" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="164"/>
-      <c r="K10" s="164"/>
+      <c r="J10" s="167"/>
+      <c r="K10" s="167"/>
     </row>
     <row r="11" spans="3:12" customFormat="1" ht="14.75" customHeight="1">
       <c r="E11" s="50"/>

</xml_diff>

<commit_message>
maj fiche agent CA
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966DCB2E-8B95-3548-A00F-6C32B028A003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2583AD-FA70-3E46-9D27-EA4B944025EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="S0xIUhd+qm/mil3mjEDLzBXqSnUj+E9UJlwfUt2w9pzFPXpGrV21CR6+VbcA2GUl+o5ORpHAcx1Tl5P1yPCQ/w==" workbookSaltValue="Ic6K1fVcoeoWgJU+jzPQ6w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19200" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille de temps" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="364">
   <si>
     <t>Temps de travail d'un magistrat</t>
   </si>
@@ -565,9 +565,6 @@
     <t>1.4.</t>
   </si>
   <si>
-    <t>AUTRES CONTENTIEUX SOCIAUX</t>
-  </si>
-  <si>
     <t>1.</t>
   </si>
   <si>
@@ -595,9 +592,6 @@
     <t>2.7.</t>
   </si>
   <si>
-    <t>TUTELLES MINEURS</t>
-  </si>
-  <si>
     <t>2.8.</t>
   </si>
   <si>
@@ -610,24 +604,12 @@
     <t>3.2.</t>
   </si>
   <si>
-    <t>PROTECTION DES MAJEURS</t>
-  </si>
-  <si>
     <t>3.3.</t>
   </si>
   <si>
-    <t>BAUX</t>
-  </si>
-  <si>
-    <t>CRÉDIT À LA CONSOMMATION</t>
-  </si>
-  <si>
     <t>3.5.</t>
   </si>
   <si>
-    <t>AUTRES CONTENTIEUX DE LA PROTECTION</t>
-  </si>
-  <si>
     <t>3.</t>
   </si>
   <si>
@@ -646,27 +628,12 @@
     <t>4.4.</t>
   </si>
   <si>
-    <t>RESPONSABILITÉ ET QUASI-CONTRATS</t>
-  </si>
-  <si>
     <t>4.5.</t>
   </si>
   <si>
-    <t>DROIT DES BIENS</t>
-  </si>
-  <si>
     <t>4.6.</t>
   </si>
   <si>
-    <t>CONSTRUCTION</t>
-  </si>
-  <si>
-    <t>DROIT DES AFFAIRES</t>
-  </si>
-  <si>
-    <t>INTÉRÊTS CIVILS</t>
-  </si>
-  <si>
     <t>CIVI</t>
   </si>
   <si>
@@ -679,39 +646,21 @@
     <t>5.1.</t>
   </si>
   <si>
-    <t>JLD CIVIL</t>
-  </si>
-  <si>
     <t>5.2.</t>
   </si>
   <si>
     <t>5.3.</t>
   </si>
   <si>
-    <t>AUTRES JLD CIVIL</t>
-  </si>
-  <si>
     <t>5.</t>
   </si>
   <si>
-    <t>TOTAL JLD CIVIL</t>
-  </si>
-  <si>
-    <t>6.1.</t>
-  </si>
-  <si>
     <t>ACTIVITÉ CIVILE</t>
   </si>
   <si>
-    <t>6.2.</t>
-  </si>
-  <si>
     <t>ACTIVITÉ PÉNALE</t>
   </si>
   <si>
-    <t>6.</t>
-  </si>
-  <si>
     <t>7.1.</t>
   </si>
   <si>
@@ -766,21 +715,9 @@
     <t>AUTRES ACTIVITÉS</t>
   </si>
   <si>
-    <t>SOUTIEN (HORS FORMATIONS SUIVIES)</t>
-  </si>
-  <si>
-    <t>FORMATIONS SUIVIES</t>
-  </si>
-  <si>
     <t>11.3.</t>
   </si>
   <si>
-    <t>FORMATIONS DISPENSÉES</t>
-  </si>
-  <si>
-    <t>ACCÈS AU DROIT ET À LA JUSTICE</t>
-  </si>
-  <si>
     <t>CSM</t>
   </si>
   <si>
@@ -1021,45 +958,12 @@
     <t>JP</t>
   </si>
   <si>
-    <t>CONTENTIEUX DU TRAVAIL</t>
-  </si>
-  <si>
-    <t>PROTECTION SOCIALE</t>
-  </si>
-  <si>
-    <t>APPEL DES RÉFÉRÉS CPH</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>COMMERCIAL</t>
   </si>
   <si>
-    <t>CONTENTIEUX COMMERCIAL GÉNÉRAL</t>
-  </si>
-  <si>
-    <t>PROCÉDURES COLLECTIVES</t>
-  </si>
-  <si>
-    <t>DROIT DES SOCIÉTÉS</t>
-  </si>
-  <si>
-    <t>CONCURRENCE</t>
-  </si>
-  <si>
-    <t>BAUX COMMERCIAUX</t>
-  </si>
-  <si>
-    <t>PROPRIÉTÉ INTELLECTUELLE ET INDUSTRIELLE</t>
-  </si>
-  <si>
-    <t>RECOURS SPÉCIFIQUES</t>
-  </si>
-  <si>
-    <t>AUTRES CONTENTIEUX COMMERCIAUX</t>
-  </si>
-  <si>
     <t>TOTAL COMMERCIAL</t>
   </si>
   <si>
@@ -1069,60 +973,27 @@
     <t>FAMILLE</t>
   </si>
   <si>
-    <t>CONTENTIEUX GÉNÉRAL DE LA FAMILLE</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX PATRIMONIAL DE LA FAMILLE</t>
-  </si>
-  <si>
-    <t>ETAT DES PERSONNES</t>
-  </si>
-  <si>
-    <t>3.4.</t>
-  </si>
-  <si>
-    <t>AUTRES CONTENTIEUX DE LA FAMILLE</t>
-  </si>
-  <si>
     <t>TOTAL FAMILLE</t>
   </si>
   <si>
     <t>PROTECTION</t>
   </si>
   <si>
-    <t>SURENDETTEMENT</t>
-  </si>
-  <si>
-    <t>APPEL DES RÉFÉRÉS DU JCP</t>
-  </si>
-  <si>
     <t>TOTAL PROTECTION</t>
   </si>
   <si>
     <t>5.4.</t>
   </si>
   <si>
-    <t>CONTENTIEUX CONTRACTUEL</t>
-  </si>
-  <si>
     <t>5.5.</t>
   </si>
   <si>
-    <t>EXPROPRIATION</t>
-  </si>
-  <si>
     <t>5.6.</t>
   </si>
   <si>
-    <t>SÛRETÉS ET EXÉCUTION</t>
-  </si>
-  <si>
     <t>5.7.</t>
   </si>
   <si>
-    <t>APPEL DES RÉFÉRÉS CIVILS</t>
-  </si>
-  <si>
     <t>5.8.</t>
   </si>
   <si>
@@ -1132,51 +1003,15 @@
     <t>5.10.</t>
   </si>
   <si>
-    <t>AUTRES CONTENTIEUX CIVILS NS</t>
-  </si>
-  <si>
-    <t>DROIT DES ÉTRANGERS</t>
-  </si>
-  <si>
-    <t>HO - CONTENTION</t>
-  </si>
-  <si>
-    <t>6.3.</t>
-  </si>
-  <si>
-    <t>VISITES DOMICILIAIRES</t>
-  </si>
-  <si>
-    <t>6.4.</t>
-  </si>
-  <si>
     <t>MINEURS</t>
   </si>
   <si>
     <t>TOTAL MINEURS</t>
   </si>
   <si>
-    <t>CORRECTIONNEL</t>
-  </si>
-  <si>
-    <t>POUVOIRS PROPRES DU PRÉSIDENT</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX GÉNÉRAL HORS JIRS</t>
-  </si>
-  <si>
-    <t>ECO-FI ET CRIM-ORG HORS JIRS</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX JIRS</t>
-  </si>
-  <si>
     <t>8.5.</t>
   </si>
   <si>
-    <t>CONTENTIEUX DU TRIBUNAL DE POLICE</t>
-  </si>
-  <si>
     <t>8.6.</t>
   </si>
   <si>
@@ -1186,114 +1021,45 @@
     <t>INSTRUCTION ET ENTRAIDE</t>
   </si>
   <si>
-    <t>CONTENTIEUX DE LA DÉTENTION HORS JIRS</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX DE LA DÉTENTION JIRS</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX DU CONTRÔLE JUDICIAIRE HORS JIRS</t>
-  </si>
-  <si>
     <t>9.5.</t>
   </si>
   <si>
-    <t>CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS</t>
-  </si>
-  <si>
     <t>9.6.</t>
   </si>
   <si>
-    <t>CONTENTIEUX DE FOND HORS JIRS</t>
-  </si>
-  <si>
     <t>9.7.</t>
   </si>
   <si>
-    <t>CONTENTIEUX DE FOND JIRS</t>
-  </si>
-  <si>
     <t>9.8.</t>
   </si>
   <si>
-    <t>ENTRAIDE PÉNALE</t>
-  </si>
-  <si>
     <t>9.9</t>
   </si>
   <si>
-    <t>CONTENTIEUX DE FOND AUTRES CONTENTIEUX SPÉCIALISÉS</t>
-  </si>
-  <si>
     <t>TOTAL INSTRUCTION ET ENTRAIDE</t>
   </si>
   <si>
     <t>APPLICATION DES PEINES</t>
   </si>
   <si>
-    <t>CHAMBRE DE L'APPLICATION DES PEINES</t>
-  </si>
-  <si>
     <t>10.3.</t>
   </si>
   <si>
-    <t>TRIBUNAL DE L'APPLICATION DES PEINES</t>
-  </si>
-  <si>
     <t>10.4.</t>
   </si>
   <si>
-    <t>JURIDICTION RÉGIONALE DES MESURES DE SÛRETÉ</t>
-  </si>
-  <si>
     <t>TOTAL APPLICATION DES PEINES</t>
   </si>
   <si>
     <t>CRIMINEL</t>
   </si>
   <si>
-    <t>ASSISES HORS JIRS</t>
-  </si>
-  <si>
     <t>11.2</t>
   </si>
   <si>
-    <t>ASSISES JIRS</t>
-  </si>
-  <si>
-    <t>COUR CRIMINELLE DÉPARTEMENTALE</t>
-  </si>
-  <si>
     <t>TOTAL CRIMINEL</t>
   </si>
   <si>
-    <t>12.1.</t>
-  </si>
-  <si>
-    <t>CONTESTATION DES HONORAIRES</t>
-  </si>
-  <si>
-    <t>12.2.</t>
-  </si>
-  <si>
-    <t>INDEMNISATION DE LA DP</t>
-  </si>
-  <si>
-    <t>12.3.</t>
-  </si>
-  <si>
-    <t>RÉFÉRÉS PP</t>
-  </si>
-  <si>
-    <t>12.4.</t>
-  </si>
-  <si>
-    <t>AUTRES ATTRIBUTIONS DU PP</t>
-  </si>
-  <si>
-    <t>12.</t>
-  </si>
-  <si>
     <t>13.1.</t>
   </si>
   <si>
@@ -1309,40 +1075,298 @@
     <t>13.5.</t>
   </si>
   <si>
-    <t>EXPERTISES (SUIVI ET LISTES)</t>
-  </si>
-  <si>
     <t>13.6.</t>
   </si>
   <si>
-    <t>MÉDIATION (SUIVI ET LISTES)</t>
-  </si>
-  <si>
     <t>13.7.</t>
   </si>
   <si>
     <t>13.8.</t>
   </si>
   <si>
-    <t>ACCUEIL DU JUSTICIABLE</t>
-  </si>
-  <si>
     <t>13.9.</t>
   </si>
   <si>
-    <t>FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL</t>
-  </si>
-  <si>
     <t>13.10.</t>
   </si>
   <si>
-    <t>AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL</t>
-  </si>
-  <si>
     <t>13.</t>
   </si>
   <si>
     <t>TOTAL PP</t>
+  </si>
+  <si>
+    <t>Contentieux du travail</t>
+  </si>
+  <si>
+    <t>Protection sociale</t>
+  </si>
+  <si>
+    <t>Appel des référés CPH</t>
+  </si>
+  <si>
+    <t>Autres contentieux sociaux</t>
+  </si>
+  <si>
+    <t>Contentieux commercial général</t>
+  </si>
+  <si>
+    <t>Procédures collectives</t>
+  </si>
+  <si>
+    <t>Droit des affaires</t>
+  </si>
+  <si>
+    <t>Droit des sociétés</t>
+  </si>
+  <si>
+    <t>Concurrence</t>
+  </si>
+  <si>
+    <t>Baux commerciaux</t>
+  </si>
+  <si>
+    <t>Propriété intellectuelle et industrielle</t>
+  </si>
+  <si>
+    <t>Recours spécifiques</t>
+  </si>
+  <si>
+    <t>Autres contentieux commerciaux</t>
+  </si>
+  <si>
+    <t>Contentieux général de la famille</t>
+  </si>
+  <si>
+    <t>Contentieux patrimonial de la famille</t>
+  </si>
+  <si>
+    <t>Etat des personnes</t>
+  </si>
+  <si>
+    <t>Autres contentieux de la famille</t>
+  </si>
+  <si>
+    <t>Protection des majeurs</t>
+  </si>
+  <si>
+    <t>Baux</t>
+  </si>
+  <si>
+    <t>Surendettement</t>
+  </si>
+  <si>
+    <t>Crédit à la consommation</t>
+  </si>
+  <si>
+    <t>Appel des référés du JCP</t>
+  </si>
+  <si>
+    <t>Autres contentieux de la protection</t>
+  </si>
+  <si>
+    <t>Tutelles mineurs</t>
+  </si>
+  <si>
+    <t>4.7.</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Autres contentieux civils NS</t>
+  </si>
+  <si>
+    <t>Droit des biens</t>
+  </si>
+  <si>
+    <t>Responsabilité et quasi-contrats</t>
+  </si>
+  <si>
+    <t>Contentieux contractuel</t>
+  </si>
+  <si>
+    <t>Expropriation</t>
+  </si>
+  <si>
+    <t>Sûretés et exécution</t>
+  </si>
+  <si>
+    <t>Appel des référés civils</t>
+  </si>
+  <si>
+    <t>Pouvoirs propres du Président</t>
+  </si>
+  <si>
+    <t>Contentieux collégial hors JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux spécialisés hors JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux JIRS crim-org</t>
+  </si>
+  <si>
+    <t>Contentieux du tribunal de Police</t>
+  </si>
+  <si>
+    <t>Intérêts civils</t>
+  </si>
+  <si>
+    <t>Contentieux JIRS éco-fi</t>
+  </si>
+  <si>
+    <t>Autres correctionnel</t>
+  </si>
+  <si>
+    <t>Contentieux à conseiller unique</t>
+  </si>
+  <si>
+    <t>8.7.</t>
+  </si>
+  <si>
+    <t>8.8.</t>
+  </si>
+  <si>
+    <t>8.9.</t>
+  </si>
+  <si>
+    <t>Autres CHINS</t>
+  </si>
+  <si>
+    <t>Contentieux de la détention hors JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux de la détention JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux de fond hors JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux de fond JIRS</t>
+  </si>
+  <si>
+    <t>Entraide pénale</t>
+  </si>
+  <si>
+    <t>Contentieux de fond contentieux spécialisés</t>
+  </si>
+  <si>
+    <t>Contentieux du contrôle judiciaire JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux du contrôle judiciaire hors JIRS</t>
+  </si>
+  <si>
+    <t>9.10.</t>
+  </si>
+  <si>
+    <t>Appels TAP</t>
+  </si>
+  <si>
+    <t>Juridiction régionale de la rétention de sûreté</t>
+  </si>
+  <si>
+    <t>Autres CHAP</t>
+  </si>
+  <si>
+    <t>Assises hors JIRS</t>
+  </si>
+  <si>
+    <t>Assises JIRS</t>
+  </si>
+  <si>
+    <t>Cour criminelle départementale</t>
+  </si>
+  <si>
+    <t>Contestation des honoraires, frais et dépens</t>
+  </si>
+  <si>
+    <t>Indemnisation de la DP</t>
+  </si>
+  <si>
+    <t>Procédures urgentes</t>
+  </si>
+  <si>
+    <t>Autres attributions du PP</t>
+  </si>
+  <si>
+    <t>Extraditions et MAE</t>
+  </si>
+  <si>
+    <t>Saisies et confiscations des avoirs criminels</t>
+  </si>
+  <si>
+    <t>Droit des étrangers</t>
+  </si>
+  <si>
+    <t>HO - Contention</t>
+  </si>
+  <si>
+    <t>Autres appels JLD</t>
+  </si>
+  <si>
+    <t>Soutien (autres)</t>
+  </si>
+  <si>
+    <t>Autres fonctionnaires / JA affectés au parquet général</t>
+  </si>
+  <si>
+    <t>Activités extérieures et partenariats</t>
+  </si>
+  <si>
+    <t>Équipement</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Politique associative et aide aux victimes</t>
+  </si>
+  <si>
+    <t>Autres activités non juridictionnelles</t>
+  </si>
+  <si>
+    <t>Formations suivies</t>
+  </si>
+  <si>
+    <t>Formations dispensées</t>
+  </si>
+  <si>
+    <t>Expertises (suivi et listes)</t>
+  </si>
+  <si>
+    <t>Médiation / conciliation (suivi et listes)</t>
+  </si>
+  <si>
+    <t>Accès au droit et à la Justice</t>
+  </si>
+  <si>
+    <t>Accueil du justiciable</t>
+  </si>
+  <si>
+    <t>Fonctionnaires / JA affectés aux activités civiles et commerciales du parquet général</t>
+  </si>
+  <si>
+    <t>13.11.</t>
+  </si>
+  <si>
+    <t>13.12.</t>
+  </si>
+  <si>
+    <t>13.13.</t>
+  </si>
+  <si>
+    <t>13.14.</t>
+  </si>
+  <si>
+    <t>13.15.</t>
+  </si>
+  <si>
+    <t>10.5.</t>
+  </si>
+  <si>
+    <t>Appels JAP</t>
   </si>
 </sst>
 </file>
@@ -1357,7 +1381,7 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1536,12 +1560,6 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1727,7 +1745,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2127,17 +2145,10 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2155,6 +2166,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2209,6 +2223,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4176,7 +4193,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE60DF7-F7D7-42C7-82AA-8FB5759BD1A1}">
   <sheetPr codeName="Feuil4"/>
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -4244,12 +4261,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="121"/>
-      <c r="B6" s="146" t="s">
+      <c r="B6" s="143" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="147"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="144"/>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
@@ -4264,7 +4281,7 @@
         <v>88</v>
       </c>
       <c r="E7" s="129">
-        <f>SUM(E13,E23,E29,E36,E47,E52,E55,E62,E72,E77,E81,E86,E97)/100</f>
+        <f>SUM(E13,E23,E28,E36,E47,E60,E70,E81,E87,E91,E57,E107)/100</f>
         <v>0</v>
       </c>
       <c r="F7" s="42"/>
@@ -4274,8 +4291,8 @@
       <c r="B8" s="130" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="148"/>
-      <c r="D8" s="149"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="131" t="s">
         <v>90</v>
       </c>
@@ -4285,11 +4302,11 @@
       <c r="A9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="142" t="s">
+      <c r="B9" s="140" t="s">
         <v>92</v>
       </c>
       <c r="C9" s="132" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="D9" s="132"/>
       <c r="E9" s="133"/>
@@ -4299,9 +4316,9 @@
       <c r="A10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="144"/>
+      <c r="B10" s="147"/>
       <c r="C10" s="132" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="D10" s="132"/>
       <c r="E10" s="133"/>
@@ -4311,9 +4328,9 @@
       <c r="A11" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="144"/>
+      <c r="B11" s="147"/>
       <c r="C11" s="132" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="D11" s="132"/>
       <c r="E11" s="133"/>
@@ -4323,9 +4340,9 @@
       <c r="A12" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="144"/>
+      <c r="B12" s="147"/>
       <c r="C12" s="132" t="s">
-        <v>96</v>
+        <v>276</v>
       </c>
       <c r="D12" s="132"/>
       <c r="E12" s="133"/>
@@ -4333,16 +4350,16 @@
     </row>
     <row r="13" spans="1:7" ht="28" customHeight="1" thickBot="1">
       <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="134" t="s">
-        <v>98</v>
-      </c>
       <c r="C13" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D13" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E13" s="136">
         <f>SUM(E9:E12)</f>
@@ -4352,13 +4369,13 @@
     </row>
     <row r="14" spans="1:7" ht="16" thickTop="1">
       <c r="A14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="142" t="s">
-        <v>252</v>
+        <v>98</v>
+      </c>
+      <c r="B14" s="140" t="s">
+        <v>228</v>
       </c>
       <c r="C14" s="132" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="D14" s="132"/>
       <c r="E14" s="133"/>
@@ -4366,11 +4383,11 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="144"/>
+        <v>101</v>
+      </c>
+      <c r="B15" s="166"/>
       <c r="C15" s="132" t="s">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="D15" s="132"/>
       <c r="E15" s="133"/>
@@ -4378,11 +4395,11 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="144"/>
+        <v>99</v>
+      </c>
+      <c r="B16" s="147"/>
       <c r="C16" s="132" t="s">
-        <v>128</v>
+        <v>278</v>
       </c>
       <c r="D16" s="132"/>
       <c r="E16" s="133"/>
@@ -4390,11 +4407,11 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="144"/>
+        <v>103</v>
+      </c>
+      <c r="B17" s="147"/>
       <c r="C17" s="132" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="D17" s="132"/>
       <c r="E17" s="133"/>
@@ -4402,11 +4419,11 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="145"/>
+        <v>100</v>
+      </c>
+      <c r="B18" s="147"/>
       <c r="C18" s="132" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
       <c r="D18" s="132"/>
       <c r="E18" s="133"/>
@@ -4416,9 +4433,9 @@
       <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="145"/>
+      <c r="B19" s="142"/>
       <c r="C19" s="132" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="D19" s="132"/>
       <c r="E19" s="133"/>
@@ -4426,11 +4443,11 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="145"/>
+        <v>102</v>
+      </c>
+      <c r="B20" s="142"/>
       <c r="C20" s="132" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="D20" s="132"/>
       <c r="E20" s="133"/>
@@ -4438,11 +4455,11 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="145"/>
+        <v>105</v>
+      </c>
+      <c r="B21" s="142"/>
       <c r="C21" s="132" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="D21" s="132"/>
       <c r="E21" s="133"/>
@@ -4450,11 +4467,11 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="145"/>
+        <v>106</v>
+      </c>
+      <c r="B22" s="142"/>
       <c r="C22" s="132" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
       <c r="D22" s="132"/>
       <c r="E22" s="133"/>
@@ -4462,16 +4479,16 @@
     </row>
     <row r="23" spans="1:6" ht="38" customHeight="1" thickBot="1">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B23" s="134" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="C23" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D23" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E23" s="136">
         <f>SUM(E14:E22)</f>
@@ -4481,13 +4498,13 @@
     </row>
     <row r="24" spans="1:6" ht="16" thickTop="1">
       <c r="A24" t="s">
-        <v>262</v>
-      </c>
-      <c r="B24" s="142" t="s">
-        <v>263</v>
+        <v>230</v>
+      </c>
+      <c r="B24" s="140" t="s">
+        <v>231</v>
       </c>
       <c r="C24" s="132" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="D24" s="132"/>
       <c r="E24" s="133"/>
@@ -4495,11 +4512,11 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="144"/>
+        <v>108</v>
+      </c>
+      <c r="B25" s="147"/>
       <c r="C25" s="132" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="D25" s="132"/>
       <c r="E25" s="133"/>
@@ -4507,11 +4524,11 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" s="144"/>
+        <v>109</v>
+      </c>
+      <c r="B26" s="147"/>
       <c r="C26" s="132" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="D26" s="132"/>
       <c r="E26" s="133"/>
@@ -4519,56 +4536,56 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>267</v>
-      </c>
-      <c r="B27" s="144"/>
+        <v>110</v>
+      </c>
+      <c r="B27" s="147"/>
       <c r="C27" s="132" t="s">
-        <v>106</v>
+        <v>289</v>
       </c>
       <c r="D27" s="132"/>
       <c r="E27" s="133"/>
       <c r="F27" s="42"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="16" thickBot="1">
       <c r="A28" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28" s="145"/>
-      <c r="C28" s="132" t="s">
-        <v>268</v>
-      </c>
-      <c r="D28" s="132"/>
-      <c r="E28" s="133"/>
+        <v>111</v>
+      </c>
+      <c r="B28" s="134" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D28" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E28" s="136">
+        <f>SUM(E24:E27)</f>
+        <v>0</v>
+      </c>
       <c r="F28" s="42"/>
     </row>
-    <row r="29" spans="1:6" ht="16" thickBot="1">
+    <row r="29" spans="1:6" ht="16" thickTop="1">
       <c r="A29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="134" t="s">
-        <v>269</v>
-      </c>
-      <c r="C29" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D29" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E29" s="136">
-        <f>SUM(E24:E28)</f>
-        <v>0</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B29" s="140" t="s">
+        <v>233</v>
+      </c>
+      <c r="C29" s="132" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="132"/>
+      <c r="E29" s="133"/>
       <c r="F29" s="42"/>
     </row>
-    <row r="30" spans="1:6" ht="16" thickTop="1">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>119</v>
-      </c>
-      <c r="B30" s="142" t="s">
-        <v>270</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="B30" s="147"/>
       <c r="C30" s="132" t="s">
-        <v>111</v>
+        <v>296</v>
       </c>
       <c r="D30" s="132"/>
       <c r="E30" s="133"/>
@@ -4576,11 +4593,11 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>120</v>
-      </c>
-      <c r="B31" s="144"/>
+        <v>115</v>
+      </c>
+      <c r="B31" s="147"/>
       <c r="C31" s="132" t="s">
-        <v>113</v>
+        <v>292</v>
       </c>
       <c r="D31" s="132"/>
       <c r="E31" s="133"/>
@@ -4588,11 +4605,11 @@
     </row>
     <row r="32" spans="1:6" ht="26" customHeight="1">
       <c r="A32" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="144"/>
+        <v>116</v>
+      </c>
+      <c r="B32" s="147"/>
       <c r="C32" s="132" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="D32" s="132"/>
       <c r="E32" s="133"/>
@@ -4600,11 +4617,11 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B33" s="144"/>
+        <v>114</v>
+      </c>
+      <c r="B33" s="147"/>
       <c r="C33" s="132" t="s">
-        <v>114</v>
+        <v>291</v>
       </c>
       <c r="D33" s="132"/>
       <c r="E33" s="133"/>
@@ -4612,11 +4629,11 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="145"/>
+        <v>117</v>
+      </c>
+      <c r="B34" s="142"/>
       <c r="C34" s="132" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="D34" s="132"/>
       <c r="E34" s="133"/>
@@ -4624,11 +4641,11 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" s="145"/>
+        <v>118</v>
+      </c>
+      <c r="B35" s="142"/>
       <c r="C35" s="132" t="s">
-        <v>116</v>
+        <v>295</v>
       </c>
       <c r="D35" s="132"/>
       <c r="E35" s="133"/>
@@ -4636,32 +4653,32 @@
     </row>
     <row r="36" spans="1:6" ht="16" thickBot="1">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B36" s="134" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="C36" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D36" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E36" s="136">
-        <f>SUM(E30:E35)</f>
+        <f>SUM(E29:E35)</f>
         <v>0</v>
       </c>
       <c r="F36" s="42"/>
     </row>
     <row r="37" spans="1:6" ht="16" thickTop="1">
       <c r="A37" t="s">
-        <v>133</v>
-      </c>
-      <c r="B37" s="142" t="s">
-        <v>118</v>
+        <v>235</v>
+      </c>
+      <c r="B37" s="140" t="s">
+        <v>112</v>
       </c>
       <c r="C37" s="132" t="s">
-        <v>127</v>
+        <v>302</v>
       </c>
       <c r="D37" s="132"/>
       <c r="E37" s="133"/>
@@ -4669,11 +4686,11 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B38" s="144"/>
+        <v>124</v>
+      </c>
+      <c r="B38" s="147"/>
       <c r="C38" s="132" t="s">
-        <v>125</v>
+        <v>301</v>
       </c>
       <c r="D38" s="132"/>
       <c r="E38" s="133"/>
@@ -4681,11 +4698,11 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" s="144"/>
+        <v>123</v>
+      </c>
+      <c r="B39" s="147"/>
       <c r="C39" s="132" t="s">
-        <v>123</v>
+        <v>300</v>
       </c>
       <c r="D39" s="132"/>
       <c r="E39" s="133"/>
@@ -4693,11 +4710,11 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B40" s="145"/>
+        <v>122</v>
+      </c>
+      <c r="B40" s="147"/>
       <c r="C40" s="132" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="D40" s="132"/>
       <c r="E40" s="133"/>
@@ -4705,11 +4722,11 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>276</v>
-      </c>
-      <c r="B41" s="145"/>
+        <v>237</v>
+      </c>
+      <c r="B41" s="147"/>
       <c r="C41" s="132" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="D41" s="132"/>
       <c r="E41" s="133"/>
@@ -4717,11 +4734,11 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>278</v>
-      </c>
-      <c r="B42" s="145"/>
+        <v>236</v>
+      </c>
+      <c r="B42" s="142"/>
       <c r="C42" s="132" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="D42" s="132"/>
       <c r="E42" s="133"/>
@@ -4729,11 +4746,11 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>280</v>
-      </c>
-      <c r="B43" s="145"/>
+        <v>238</v>
+      </c>
+      <c r="B43" s="142"/>
       <c r="C43" s="132" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="D43" s="132"/>
       <c r="E43" s="133"/>
@@ -4741,11 +4758,11 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>282</v>
-      </c>
-      <c r="B44" s="145"/>
+        <v>239</v>
+      </c>
+      <c r="B44" s="142"/>
       <c r="C44" s="132" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D44" s="132"/>
       <c r="E44" s="133"/>
@@ -4753,11 +4770,11 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>283</v>
-      </c>
-      <c r="B45" s="145"/>
+        <v>240</v>
+      </c>
+      <c r="B45" s="142"/>
       <c r="C45" s="132" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="D45" s="132"/>
       <c r="E45" s="133"/>
@@ -4765,11 +4782,11 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>284</v>
-      </c>
-      <c r="B46" s="145"/>
+        <v>241</v>
+      </c>
+      <c r="B46" s="142"/>
       <c r="C46" s="132" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="D46" s="132"/>
       <c r="E46" s="133"/>
@@ -4777,16 +4794,16 @@
     </row>
     <row r="47" spans="1:6" ht="16" thickBot="1">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B47" s="134" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C47" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D47" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E47" s="136">
         <f>SUM(E37:E46)</f>
@@ -4795,152 +4812,113 @@
       <c r="F47" s="42"/>
     </row>
     <row r="48" spans="1:6" ht="16" thickTop="1">
-      <c r="A48" t="s">
-        <v>140</v>
-      </c>
-      <c r="B48" s="142" t="s">
-        <v>134</v>
+      <c r="B48" s="140" t="s">
+        <v>204</v>
       </c>
       <c r="C48" s="132" t="s">
-        <v>286</v>
+        <v>334</v>
       </c>
       <c r="D48" s="132"/>
       <c r="E48" s="133"/>
       <c r="F48" s="42"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>142</v>
-      </c>
-      <c r="B49" s="144"/>
+      <c r="B49" s="166"/>
       <c r="C49" s="132" t="s">
-        <v>287</v>
+        <v>335</v>
       </c>
       <c r="D49" s="132"/>
       <c r="E49" s="133"/>
       <c r="F49" s="42"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>288</v>
-      </c>
-      <c r="B50" s="144"/>
+      <c r="B50" s="166"/>
       <c r="C50" s="132" t="s">
-        <v>289</v>
+        <v>336</v>
       </c>
       <c r="D50" s="132"/>
       <c r="E50" s="133"/>
       <c r="F50" s="42"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>290</v>
-      </c>
-      <c r="B51" s="144"/>
+      <c r="B51" s="166"/>
       <c r="C51" s="132" t="s">
-        <v>137</v>
+        <v>337</v>
       </c>
       <c r="D51" s="132"/>
       <c r="E51" s="133"/>
       <c r="F51" s="42"/>
     </row>
-    <row r="52" spans="1:6" ht="33" customHeight="1" thickBot="1">
-      <c r="A52" t="s">
-        <v>144</v>
-      </c>
-      <c r="B52" s="134" t="s">
-        <v>139</v>
-      </c>
-      <c r="C52" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D52" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E52" s="136">
-        <f>SUM(E48:E51)</f>
-        <v>0</v>
-      </c>
+    <row r="52" spans="1:6">
+      <c r="B52" s="166"/>
+      <c r="C52" s="132" t="s">
+        <v>338</v>
+      </c>
+      <c r="D52" s="132"/>
+      <c r="E52" s="133"/>
       <c r="F52" s="42"/>
     </row>
-    <row r="53" spans="1:6" ht="16" thickTop="1">
-      <c r="A53" t="s">
-        <v>145</v>
-      </c>
-      <c r="B53" s="142" t="s">
-        <v>291</v>
-      </c>
+    <row r="53" spans="1:6">
+      <c r="B53" s="141"/>
       <c r="C53" s="132" t="s">
-        <v>141</v>
+        <v>339</v>
       </c>
       <c r="D53" s="132"/>
       <c r="E53" s="133"/>
       <c r="F53" s="42"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>146</v>
-      </c>
-      <c r="B54" s="143"/>
+      <c r="B54" s="141"/>
       <c r="C54" s="132" t="s">
-        <v>143</v>
+        <v>340</v>
       </c>
       <c r="D54" s="132"/>
       <c r="E54" s="133"/>
       <c r="F54" s="42"/>
     </row>
-    <row r="55" spans="1:6" ht="16" thickBot="1">
-      <c r="A55" t="s">
-        <v>147</v>
-      </c>
-      <c r="B55" s="134" t="s">
-        <v>292</v>
-      </c>
-      <c r="C55" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D55" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E55" s="136">
-        <f>SUM(E53:E54)</f>
-        <v>0</v>
-      </c>
+    <row r="55" spans="1:6">
+      <c r="B55" s="141"/>
+      <c r="C55" s="132" t="s">
+        <v>341</v>
+      </c>
+      <c r="D55" s="132"/>
+      <c r="E55" s="133"/>
       <c r="F55" s="42"/>
     </row>
-    <row r="56" spans="1:6" ht="16" thickTop="1">
-      <c r="A56" t="s">
-        <v>148</v>
-      </c>
-      <c r="B56" s="142" t="s">
-        <v>293</v>
-      </c>
+    <row r="56" spans="1:6">
+      <c r="B56" s="142"/>
       <c r="C56" s="132" t="s">
-        <v>294</v>
+        <v>342</v>
       </c>
       <c r="D56" s="132"/>
       <c r="E56" s="133"/>
       <c r="F56" s="42"/>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>149</v>
-      </c>
-      <c r="B57" s="144"/>
-      <c r="C57" s="132" t="s">
-        <v>295</v>
-      </c>
-      <c r="D57" s="132"/>
-      <c r="E57" s="133"/>
+    <row r="57" spans="1:6" ht="16" thickBot="1">
+      <c r="B57" s="134" t="s">
+        <v>272</v>
+      </c>
+      <c r="C57" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D57" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E57" s="136">
+        <f>SUM(E48:E56)</f>
+        <v>0</v>
+      </c>
       <c r="F57" s="42"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" ht="16" thickTop="1">
       <c r="A58" t="s">
-        <v>150</v>
-      </c>
-      <c r="B58" s="144"/>
+        <v>128</v>
+      </c>
+      <c r="B58" s="140" t="s">
+        <v>242</v>
+      </c>
       <c r="C58" s="132" t="s">
-        <v>296</v>
+        <v>126</v>
       </c>
       <c r="D58" s="132"/>
       <c r="E58" s="133"/>
@@ -4948,68 +4926,66 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>151</v>
-      </c>
-      <c r="B59" s="144"/>
+        <v>129</v>
+      </c>
+      <c r="B59" s="141"/>
       <c r="C59" s="132" t="s">
-        <v>297</v>
+        <v>127</v>
       </c>
       <c r="D59" s="132"/>
       <c r="E59" s="133"/>
       <c r="F59" s="42"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" ht="16" thickBot="1">
       <c r="A60" t="s">
-        <v>298</v>
-      </c>
-      <c r="B60" s="145"/>
-      <c r="C60" s="132" t="s">
-        <v>299</v>
-      </c>
-      <c r="D60" s="132"/>
-      <c r="E60" s="133"/>
+        <v>130</v>
+      </c>
+      <c r="B60" s="134" t="s">
+        <v>243</v>
+      </c>
+      <c r="C60" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D60" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E60" s="136">
+        <f>SUM(E58:E59)</f>
+        <v>0</v>
+      </c>
       <c r="F60" s="42"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" ht="16" thickTop="1">
       <c r="A61" t="s">
-        <v>300</v>
-      </c>
-      <c r="B61" s="145"/>
+        <v>131</v>
+      </c>
+      <c r="B61" s="166"/>
       <c r="C61" s="132" t="s">
-        <v>129</v>
+        <v>306</v>
       </c>
       <c r="D61" s="132"/>
       <c r="E61" s="133"/>
       <c r="F61" s="42"/>
     </row>
-    <row r="62" spans="1:6" ht="16" thickBot="1">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>152</v>
-      </c>
-      <c r="B62" s="134" t="s">
-        <v>301</v>
-      </c>
-      <c r="C62" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D62" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E62" s="136">
-        <f>SUM(E56:E61)</f>
-        <v>0</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="B62" s="147"/>
+      <c r="C62" s="132" t="s">
+        <v>307</v>
+      </c>
+      <c r="D62" s="132"/>
+      <c r="E62" s="133"/>
       <c r="F62" s="42"/>
     </row>
-    <row r="63" spans="1:6" ht="16" thickTop="1">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>153</v>
-      </c>
-      <c r="B63" s="142" t="s">
-        <v>302</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="B63" s="147"/>
       <c r="C63" s="132" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="D63" s="132"/>
       <c r="E63" s="133"/>
@@ -5017,11 +4993,11 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>154</v>
-      </c>
-      <c r="B64" s="144"/>
+        <v>134</v>
+      </c>
+      <c r="B64" s="147"/>
       <c r="C64" s="132" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="D64" s="132"/>
       <c r="E64" s="133"/>
@@ -5029,11 +5005,11 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>155</v>
-      </c>
-      <c r="B65" s="144"/>
+        <v>315</v>
+      </c>
+      <c r="B65" s="147"/>
       <c r="C65" s="132" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="D65" s="132"/>
       <c r="E65" s="133"/>
@@ -5041,11 +5017,11 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>156</v>
-      </c>
-      <c r="B66" s="144"/>
+        <v>317</v>
+      </c>
+      <c r="B66" s="147"/>
       <c r="C66" s="132" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="D66" s="132"/>
       <c r="E66" s="133"/>
@@ -5053,11 +5029,11 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>306</v>
-      </c>
-      <c r="B67" s="145"/>
+        <v>244</v>
+      </c>
+      <c r="B67" s="142"/>
       <c r="C67" s="132" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D67" s="132"/>
       <c r="E67" s="133"/>
@@ -5065,11 +5041,11 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>308</v>
-      </c>
-      <c r="B68" s="145"/>
+        <v>245</v>
+      </c>
+      <c r="B68" s="142"/>
       <c r="C68" s="132" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D68" s="132"/>
       <c r="E68" s="133"/>
@@ -5077,68 +5053,68 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>310</v>
-      </c>
-      <c r="B69" s="145"/>
+        <v>316</v>
+      </c>
+      <c r="B69" s="142"/>
       <c r="C69" s="132" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D69" s="132"/>
       <c r="E69" s="133"/>
       <c r="F69" s="42"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" ht="16" thickBot="1">
       <c r="A70" t="s">
-        <v>312</v>
-      </c>
-      <c r="B70" s="145"/>
-      <c r="C70" s="132" t="s">
-        <v>313</v>
-      </c>
-      <c r="D70" s="132"/>
-      <c r="E70" s="133"/>
+        <v>135</v>
+      </c>
+      <c r="B70" s="134" t="s">
+        <v>246</v>
+      </c>
+      <c r="C70" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D70" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E70" s="136">
+        <f>SUM(E61:E69)</f>
+        <v>0</v>
+      </c>
       <c r="F70" s="42"/>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" ht="16" thickTop="1">
       <c r="A71" t="s">
-        <v>314</v>
-      </c>
-      <c r="B71" s="145"/>
+        <v>136</v>
+      </c>
+      <c r="B71" s="140" t="s">
+        <v>247</v>
+      </c>
       <c r="C71" s="132" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="D71" s="132"/>
       <c r="E71" s="133"/>
       <c r="F71" s="42"/>
     </row>
-    <row r="72" spans="1:6" ht="16" thickBot="1">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>157</v>
-      </c>
-      <c r="B72" s="134" t="s">
-        <v>316</v>
-      </c>
-      <c r="C72" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D72" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E72" s="136">
-        <f>SUM(E63:E71)</f>
-        <v>0</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="B72" s="147"/>
+      <c r="C72" s="132" t="s">
+        <v>319</v>
+      </c>
+      <c r="D72" s="132"/>
+      <c r="E72" s="133"/>
       <c r="F72" s="42"/>
     </row>
-    <row r="73" spans="1:6" ht="16" thickTop="1">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>158</v>
-      </c>
-      <c r="B73" s="142" t="s">
-        <v>317</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B73" s="147"/>
       <c r="C73" s="132" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="D73" s="132"/>
       <c r="E73" s="133"/>
@@ -5146,11 +5122,11 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>159</v>
-      </c>
-      <c r="B74" s="144"/>
+        <v>139</v>
+      </c>
+      <c r="B74" s="142"/>
       <c r="C74" s="132" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="D74" s="132"/>
       <c r="E74" s="133"/>
@@ -5158,11 +5134,11 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>319</v>
-      </c>
-      <c r="B75" s="144"/>
+        <v>248</v>
+      </c>
+      <c r="B75" s="142"/>
       <c r="C75" s="132" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="D75" s="132"/>
       <c r="E75" s="133"/>
@@ -5170,44 +5146,35 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
+        <v>249</v>
+      </c>
+      <c r="B76" s="142"/>
+      <c r="C76" s="132" t="s">
         <v>321</v>
-      </c>
-      <c r="B76" s="144"/>
-      <c r="C76" s="132" t="s">
-        <v>322</v>
       </c>
       <c r="D76" s="132"/>
       <c r="E76" s="133"/>
       <c r="F76" s="42"/>
     </row>
-    <row r="77" spans="1:6" ht="16" thickBot="1">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>160</v>
-      </c>
-      <c r="B77" s="134" t="s">
-        <v>323</v>
-      </c>
-      <c r="C77" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D77" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E77" s="136">
-        <f>SUM(E73:E76)</f>
-        <v>0</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="B77" s="142"/>
+      <c r="C77" s="132" t="s">
+        <v>322</v>
+      </c>
+      <c r="D77" s="132"/>
+      <c r="E77" s="133"/>
       <c r="F77" s="42"/>
     </row>
-    <row r="78" spans="1:6" ht="16" thickTop="1">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>161</v>
-      </c>
-      <c r="B78" s="142" t="s">
+        <v>252</v>
+      </c>
+      <c r="B78" s="142"/>
+      <c r="C78" s="132" t="s">
         <v>324</v>
-      </c>
-      <c r="C78" s="132" t="s">
-        <v>325</v>
       </c>
       <c r="D78" s="132"/>
       <c r="E78" s="133"/>
@@ -5215,11 +5182,11 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>326</v>
-      </c>
-      <c r="B79" s="143"/>
+        <v>251</v>
+      </c>
+      <c r="B79" s="142"/>
       <c r="C79" s="132" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D79" s="132"/>
       <c r="E79" s="133"/>
@@ -5227,11 +5194,11 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>165</v>
-      </c>
-      <c r="B80" s="143"/>
+        <v>327</v>
+      </c>
+      <c r="B80" s="142"/>
       <c r="C80" s="132" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="D80" s="132"/>
       <c r="E80" s="133"/>
@@ -5239,32 +5206,32 @@
     </row>
     <row r="81" spans="1:6" ht="16" thickBot="1">
       <c r="A81" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="B81" s="134" t="s">
-        <v>329</v>
+        <v>253</v>
       </c>
       <c r="C81" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D81" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E81" s="136">
-        <f>SUM(E78:E80)</f>
+        <f>SUM(E71:E80)</f>
         <v>0</v>
       </c>
       <c r="F81" s="42"/>
     </row>
     <row r="82" spans="1:6" ht="16" thickTop="1">
       <c r="A82" t="s">
-        <v>330</v>
-      </c>
-      <c r="B82" s="142" t="s">
-        <v>225</v>
+        <v>141</v>
+      </c>
+      <c r="B82" s="140" t="s">
+        <v>254</v>
       </c>
       <c r="C82" s="132" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
       <c r="D82" s="132"/>
       <c r="E82" s="133"/>
@@ -5272,11 +5239,11 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>332</v>
-      </c>
-      <c r="B83" s="143"/>
+        <v>142</v>
+      </c>
+      <c r="B83" s="147"/>
       <c r="C83" s="132" t="s">
-        <v>333</v>
+        <v>363</v>
       </c>
       <c r="D83" s="132"/>
       <c r="E83" s="133"/>
@@ -5284,11 +5251,11 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>334</v>
-      </c>
-      <c r="B84" s="143"/>
+        <v>255</v>
+      </c>
+      <c r="B84" s="147"/>
       <c r="C84" s="132" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D84" s="132"/>
       <c r="E84" s="133"/>
@@ -5296,56 +5263,56 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>336</v>
-      </c>
-      <c r="B85" s="145"/>
+        <v>256</v>
+      </c>
+      <c r="B85" s="147"/>
       <c r="C85" s="132" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D85" s="132"/>
       <c r="E85" s="133"/>
       <c r="F85" s="42"/>
     </row>
-    <row r="86" spans="1:6" ht="16" thickBot="1">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>338</v>
-      </c>
-      <c r="B86" s="134" t="s">
-        <v>355</v>
-      </c>
-      <c r="C86" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D86" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E86" s="136">
-        <f>SUM(E82:E85)</f>
+        <v>362</v>
+      </c>
+      <c r="B86" s="147"/>
+      <c r="C86" s="132" t="s">
+        <v>330</v>
+      </c>
+      <c r="D86" s="132"/>
+      <c r="E86" s="133"/>
+      <c r="F86" s="42"/>
+    </row>
+    <row r="87" spans="1:6" ht="16" thickBot="1">
+      <c r="A87" t="s">
+        <v>143</v>
+      </c>
+      <c r="B87" s="134" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D87" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E87" s="136">
+        <f>SUM(E82:E86)</f>
         <v>0</v>
       </c>
-      <c r="F86" s="42"/>
-    </row>
-    <row r="87" spans="1:6" ht="16" thickTop="1">
-      <c r="A87" t="s">
-        <v>339</v>
-      </c>
-      <c r="B87" s="142" t="s">
-        <v>162</v>
-      </c>
-      <c r="C87" s="132" t="s">
-        <v>163</v>
-      </c>
-      <c r="D87" s="132"/>
-      <c r="E87" s="133"/>
       <c r="F87" s="42"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" ht="16" thickTop="1">
       <c r="A88" t="s">
-        <v>340</v>
-      </c>
-      <c r="B88" s="143"/>
+        <v>144</v>
+      </c>
+      <c r="B88" s="140" t="s">
+        <v>258</v>
+      </c>
       <c r="C88" s="132" t="s">
-        <v>164</v>
+        <v>331</v>
       </c>
       <c r="D88" s="132"/>
       <c r="E88" s="133"/>
@@ -5353,11 +5320,11 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>341</v>
-      </c>
-      <c r="B89" s="145"/>
+        <v>259</v>
+      </c>
+      <c r="B89" s="141"/>
       <c r="C89" s="132" t="s">
-        <v>166</v>
+        <v>332</v>
       </c>
       <c r="D89" s="132"/>
       <c r="E89" s="133"/>
@@ -5365,35 +5332,44 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>342</v>
-      </c>
-      <c r="B90" s="145"/>
+        <v>146</v>
+      </c>
+      <c r="B90" s="141"/>
       <c r="C90" s="132" t="s">
-        <v>168</v>
+        <v>333</v>
       </c>
       <c r="D90" s="132"/>
       <c r="E90" s="133"/>
       <c r="F90" s="42"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" ht="16" thickBot="1">
       <c r="A91" t="s">
-        <v>343</v>
-      </c>
-      <c r="B91" s="145"/>
-      <c r="C91" s="132" t="s">
-        <v>344</v>
-      </c>
-      <c r="D91" s="132"/>
-      <c r="E91" s="133"/>
+        <v>148</v>
+      </c>
+      <c r="B91" s="134" t="s">
+        <v>260</v>
+      </c>
+      <c r="C91" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D91" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E91" s="136">
+        <f>SUM(E88:E90)</f>
+        <v>0</v>
+      </c>
       <c r="F91" s="42"/>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" ht="16" thickTop="1">
       <c r="A92" t="s">
-        <v>345</v>
-      </c>
-      <c r="B92" s="145"/>
+        <v>267</v>
+      </c>
+      <c r="B92" s="140" t="s">
+        <v>145</v>
+      </c>
       <c r="C92" s="132" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="D92" s="132"/>
       <c r="E92" s="133"/>
@@ -5401,11 +5377,11 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>347</v>
-      </c>
-      <c r="B93" s="145"/>
+        <v>268</v>
+      </c>
+      <c r="B93" s="166"/>
       <c r="C93" s="132" t="s">
-        <v>167</v>
+        <v>355</v>
       </c>
       <c r="D93" s="132"/>
       <c r="E93" s="133"/>
@@ -5413,99 +5389,218 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>348</v>
-      </c>
-      <c r="B94" s="145"/>
+        <v>357</v>
+      </c>
+      <c r="B94" s="166"/>
       <c r="C94" s="132" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D94" s="132"/>
       <c r="E94" s="133"/>
       <c r="F94" s="42"/>
     </row>
-    <row r="95" spans="1:6" s="141" customFormat="1" ht="38" customHeight="1">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>350</v>
-      </c>
-      <c r="B95" s="145"/>
+        <v>359</v>
+      </c>
+      <c r="B95" s="166"/>
       <c r="C95" s="132" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D95" s="132"/>
       <c r="E95" s="133"/>
-      <c r="F95" s="140"/>
-    </row>
-    <row r="96" spans="1:6" ht="30">
+      <c r="F95" s="42"/>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>352</v>
-      </c>
-      <c r="B96" s="145"/>
+        <v>264</v>
+      </c>
+      <c r="B96" s="166"/>
       <c r="C96" s="132" t="s">
-        <v>353</v>
+        <v>147</v>
       </c>
       <c r="D96" s="132"/>
       <c r="E96" s="133"/>
       <c r="F96" s="42"/>
     </row>
-    <row r="97" spans="1:6" ht="16" thickBot="1">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>354</v>
-      </c>
-      <c r="B97" s="134" t="s">
-        <v>170</v>
-      </c>
-      <c r="C97" s="135"/>
-      <c r="D97" s="135"/>
-      <c r="E97" s="136">
-        <f>SUM(E87:E96)</f>
+        <v>358</v>
+      </c>
+      <c r="B97" s="166"/>
+      <c r="C97" s="132" t="s">
+        <v>346</v>
+      </c>
+      <c r="D97" s="132"/>
+      <c r="E97" s="133"/>
+      <c r="F97" s="42"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>265</v>
+      </c>
+      <c r="B98" s="166"/>
+      <c r="C98" s="132" t="s">
+        <v>352</v>
+      </c>
+      <c r="D98" s="132"/>
+      <c r="E98" s="133"/>
+      <c r="F98" s="42"/>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>262</v>
+      </c>
+      <c r="B99" s="166"/>
+      <c r="C99" s="132" t="s">
+        <v>350</v>
+      </c>
+      <c r="D99" s="132"/>
+      <c r="E99" s="133"/>
+      <c r="F99" s="42"/>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>263</v>
+      </c>
+      <c r="B100" s="166"/>
+      <c r="C100" s="132" t="s">
+        <v>351</v>
+      </c>
+      <c r="D100" s="132"/>
+      <c r="E100" s="133"/>
+      <c r="F100" s="42"/>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" t="s">
+        <v>266</v>
+      </c>
+      <c r="B101" s="166"/>
+      <c r="C101" s="132" t="s">
+        <v>353</v>
+      </c>
+      <c r="D101" s="132"/>
+      <c r="E101" s="133"/>
+      <c r="F101" s="42"/>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" t="s">
+        <v>360</v>
+      </c>
+      <c r="B102" s="142"/>
+      <c r="C102" s="132" t="s">
+        <v>348</v>
+      </c>
+      <c r="D102" s="132"/>
+      <c r="E102" s="133"/>
+      <c r="F102" s="42"/>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" t="s">
+        <v>261</v>
+      </c>
+      <c r="B103" s="142"/>
+      <c r="C103" s="132" t="s">
+        <v>343</v>
+      </c>
+      <c r="D103" s="132"/>
+      <c r="E103" s="133"/>
+      <c r="F103" s="42"/>
+    </row>
+    <row r="104" spans="1:6" ht="30">
+      <c r="A104" t="s">
+        <v>269</v>
+      </c>
+      <c r="B104" s="142"/>
+      <c r="C104" s="132" t="s">
+        <v>356</v>
+      </c>
+      <c r="D104" s="132"/>
+      <c r="E104" s="133"/>
+      <c r="F104" s="42"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
+        <v>270</v>
+      </c>
+      <c r="B105" s="142"/>
+      <c r="C105" s="132" t="s">
+        <v>344</v>
+      </c>
+      <c r="D105" s="132"/>
+      <c r="E105" s="133"/>
+      <c r="F105" s="42"/>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
+        <v>361</v>
+      </c>
+      <c r="B106" s="142"/>
+      <c r="C106" s="132" t="s">
+        <v>349</v>
+      </c>
+      <c r="D106" s="132"/>
+      <c r="E106" s="133"/>
+      <c r="F106" s="42"/>
+    </row>
+    <row r="107" spans="1:6" ht="16" thickBot="1">
+      <c r="A107" t="s">
+        <v>271</v>
+      </c>
+      <c r="B107" s="134" t="s">
+        <v>149</v>
+      </c>
+      <c r="C107" s="135"/>
+      <c r="D107" s="135"/>
+      <c r="E107" s="136">
+        <f>SUM(E92:E106)</f>
         <v>0</v>
       </c>
-      <c r="F97" s="42"/>
-    </row>
-    <row r="98" spans="1:6" ht="16" thickTop="1">
-      <c r="A98" s="10"/>
-      <c r="F98" s="42"/>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="10"/>
-      <c r="F99" s="42"/>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="10"/>
-      <c r="F100" s="42"/>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="10"/>
-      <c r="F101" s="42"/>
-    </row>
-    <row r="102" spans="1:6" ht="23" customHeight="1">
-      <c r="A102" s="10"/>
-      <c r="F102" s="42"/>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103" s="10"/>
-      <c r="F103" s="42"/>
-    </row>
-    <row r="104" spans="1:6" ht="98" hidden="1" customHeight="1"/>
+      <c r="F107" s="42"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="10"/>
+      <c r="F108" s="42"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="10"/>
+      <c r="F109" s="42"/>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="10"/>
+      <c r="F110" s="42"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="10"/>
+      <c r="F111" s="42"/>
+    </row>
+    <row r="112" spans="1:6" ht="23" customHeight="1">
+      <c r="A112" s="10"/>
+      <c r="F112" s="42"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="10"/>
+      <c r="F113" s="42"/>
+    </row>
+    <row r="114" spans="1:6" ht="98" hidden="1" customHeight="1"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="1b5cR/Y9gE1aCr4AZysTr2nkvHi+VUlUqFo95Xb2iAselYPtX7csV35FQfkFR4Dq/34I5Up+zbOh3kFgt3nfkA==" saltValue="dBSUhmRnhYZe8qrAXcguXA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+RPmeKs/hifhcslRmMk7+9Ww7GK4vT0NQ+S3QLLK9lcGwt/InRX3vHxeJhDSEDX477Sr23lVwwaaXC8XKsGRfg==" saltValue="ALl5IvnyvjSs2ArDqFY0eg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
-  <mergeCells count="15">
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B87:B96"/>
+  <mergeCells count="14">
+    <mergeCell ref="B48:B56"/>
+    <mergeCell ref="B92:B106"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="B14:B22"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B37:B46"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="B63:B71"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B61:B69"/>
+    <mergeCell ref="B71:B80"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="B88:B90"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A12">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -5564,32 +5659,32 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="137" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="B1" s="137" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="C1" s="138" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="E1" s="137" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="F1" s="137" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G1" s="138" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="H1" s="138"/>
       <c r="I1" s="137" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="J1" s="137" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="K1" s="138" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="M1" t="s">
         <v>50</v>
@@ -5597,92 +5692,92 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="C2" s="139">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="J2" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="K2">
         <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="C3" s="139">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="F3" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="J3" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="K3">
         <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="C4" s="139">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="F4" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="J4" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="K4">
         <v>3</v>
@@ -5690,28 +5785,28 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="C5" s="139">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="F5" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="J5" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -5719,28 +5814,28 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="C6" s="139">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="J6" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -5748,28 +5843,28 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="C7" s="139">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="F7" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="J7" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="K7">
         <v>3</v>
@@ -5777,28 +5872,28 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="C8" s="139">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="J8" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="K8">
         <v>3</v>
@@ -5806,19 +5901,19 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="C9" s="139">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="F9" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -5826,19 +5921,19 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C10" s="139">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="F10" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -5846,19 +5941,19 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="C11" s="139">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="F11" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -5866,19 +5961,19 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="C12" s="139">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -5887,10 +5982,10 @@
     <row r="13" spans="1:13">
       <c r="C13" s="139"/>
       <c r="E13" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="F13" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -5899,10 +5994,10 @@
     <row r="14" spans="1:13">
       <c r="C14" s="139"/>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="F14" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -5911,10 +6006,10 @@
     <row r="15" spans="1:13">
       <c r="C15" s="139"/>
       <c r="E15" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="F15" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -5923,10 +6018,10 @@
     <row r="16" spans="1:13">
       <c r="C16" s="139"/>
       <c r="E16" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="F16" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -5935,10 +6030,10 @@
     <row r="17" spans="3:7">
       <c r="C17" s="139"/>
       <c r="E17" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="F17" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -5947,10 +6042,10 @@
     <row r="18" spans="3:7">
       <c r="C18" s="139"/>
       <c r="E18" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F18" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -5959,10 +6054,10 @@
     <row r="19" spans="3:7">
       <c r="C19" s="139"/>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="F19" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -5971,10 +6066,10 @@
     <row r="20" spans="3:7">
       <c r="C20" s="139"/>
       <c r="E20" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="F20" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="G20">
         <v>2</v>
@@ -5983,10 +6078,10 @@
     <row r="21" spans="3:7">
       <c r="C21" s="139"/>
       <c r="E21" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="F21" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="G21">
         <v>2</v>
@@ -5995,10 +6090,10 @@
     <row r="22" spans="3:7">
       <c r="C22" s="139"/>
       <c r="E22" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="F22" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -6007,10 +6102,10 @@
     <row r="23" spans="3:7">
       <c r="C23" s="139"/>
       <c r="E23" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="F23" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="G23">
         <v>2</v>
@@ -6019,10 +6114,10 @@
     <row r="24" spans="3:7">
       <c r="C24" s="139"/>
       <c r="E24" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="F24" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="G24">
         <v>2</v>
@@ -6031,10 +6126,10 @@
     <row r="25" spans="3:7">
       <c r="C25" s="139"/>
       <c r="E25" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="F25" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="G25">
         <v>2</v>
@@ -6043,10 +6138,10 @@
     <row r="26" spans="3:7">
       <c r="C26" s="139"/>
       <c r="E26" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="F26" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="G26">
         <v>2</v>
@@ -6124,10 +6219,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="27"/>
-      <c r="F4" s="155" t="s">
+      <c r="F4" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="156"/>
+      <c r="G4" s="154"/>
       <c r="H4" s="71"/>
       <c r="I4" s="2">
         <v>208</v>
@@ -6138,10 +6233,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="F5" s="157" t="s">
+      <c r="F5" s="155" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="158"/>
+      <c r="G5" s="156"/>
       <c r="H5" s="72"/>
       <c r="I5" s="6">
         <v>8</v>
@@ -6157,28 +6252,28 @@
       <c r="H6" s="35"/>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="153" t="s">
+      <c r="B7" s="151" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="152" t="s">
+      <c r="E7" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="152"/>
+      <c r="F7" s="150"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="150" t="s">
+      <c r="I7" s="148" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="69"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="154"/>
-      <c r="I8" s="151"/>
+      <c r="B8" s="152"/>
+      <c r="I8" s="149"/>
       <c r="J8" s="70"/>
       <c r="L8"/>
     </row>
@@ -6220,7 +6315,7 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="153" t="s">
+      <c r="B12" s="151" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="32" t="s">
@@ -6236,11 +6331,11 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="154"/>
+      <c r="B13" s="152"/>
       <c r="C13" s="77"/>
       <c r="D13" s="77"/>
       <c r="E13" s="73"/>
-      <c r="G13" s="151" t="s">
+      <c r="G13" s="149" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="70"/>
@@ -6255,7 +6350,7 @@
       <c r="E14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="151"/>
+      <c r="G14" s="149"/>
       <c r="H14" s="70"/>
       <c r="I14" s="10"/>
     </row>
@@ -6385,14 +6480,14 @@
       </c>
       <c r="C3" s="114"/>
       <c r="D3" s="26"/>
-      <c r="F3" s="159" t="s">
+      <c r="F3" s="157" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="161"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="159"/>
       <c r="L3"/>
     </row>
     <row r="4" spans="2:12" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
@@ -6401,10 +6496,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="27"/>
-      <c r="F4" s="155" t="s">
+      <c r="F4" s="153" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="156"/>
+      <c r="G4" s="154"/>
       <c r="H4" s="71"/>
       <c r="I4" s="10">
         <v>1607</v>
@@ -6415,10 +6510,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="F5" s="157" t="s">
+      <c r="F5" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="158"/>
+      <c r="G5" s="156"/>
       <c r="H5" s="72"/>
       <c r="I5" s="104">
         <v>35</v>
@@ -6435,28 +6530,28 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="153" t="s">
+      <c r="B7" s="151" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="152" t="s">
+      <c r="E7" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="152"/>
+      <c r="F7" s="150"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="150" t="s">
+      <c r="I7" s="148" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="69"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="154"/>
-      <c r="I8" s="151"/>
+      <c r="B8" s="152"/>
+      <c r="I8" s="149"/>
       <c r="J8" s="70"/>
       <c r="L8"/>
     </row>
@@ -6499,7 +6594,7 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="153" t="s">
+      <c r="B12" s="151" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="118" t="s">
@@ -6515,11 +6610,11 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="154"/>
+      <c r="B13" s="152"/>
       <c r="C13" s="119"/>
       <c r="D13" s="77"/>
       <c r="E13" s="73"/>
-      <c r="G13" s="151" t="s">
+      <c r="G13" s="149" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="70"/>
@@ -6534,7 +6629,7 @@
       <c r="E14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="151"/>
+      <c r="G14" s="149"/>
       <c r="H14" s="70"/>
       <c r="I14" s="10"/>
     </row>
@@ -6650,30 +6745,30 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="3:9" ht="54.75" customHeight="1">
-      <c r="C2" s="163" t="s">
+      <c r="C2" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="161"/>
+      <c r="G2" s="161"/>
+      <c r="H2" s="161"/>
+      <c r="I2" s="161"/>
     </row>
     <row r="3" spans="3:9" ht="27.75" customHeight="1">
       <c r="C3" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="162" t="s">
+      <c r="D3" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="162"/>
-      <c r="F3" s="164" t="s">
+      <c r="E3" s="160"/>
+      <c r="F3" s="162" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="164"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="164"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
     </row>
     <row r="4" spans="3:9" ht="23.25" customHeight="1">
       <c r="C4" s="40" t="s">
@@ -6929,26 +7024,26 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="3:12" ht="46.5" customHeight="1">
-      <c r="E2" s="165" t="s">
+      <c r="E2" s="163" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="163"/>
+      <c r="K2" s="163"/>
     </row>
     <row r="3" spans="3:12" ht="53.25" customHeight="1">
-      <c r="E3" s="166" t="s">
+      <c r="E3" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="F3" s="164"/>
+      <c r="G3" s="164"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="164"/>
+      <c r="J3" s="164"/>
+      <c r="K3" s="164"/>
     </row>
     <row r="4" spans="3:12" ht="20.75" customHeight="1">
       <c r="E4" s="61"/>
@@ -7007,10 +7102,10 @@
       <c r="I8" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="164" t="s">
+      <c r="J8" s="162" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="164"/>
+      <c r="K8" s="162"/>
     </row>
     <row r="9" spans="3:12" ht="14" customHeight="1">
       <c r="D9" s="39"/>
@@ -7030,11 +7125,11 @@
       <c r="H10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="167" t="s">
+      <c r="I10" s="165" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="167"/>
-      <c r="K10" s="167"/>
+      <c r="J10" s="165"/>
+      <c r="K10" s="165"/>
     </row>
     <row r="11" spans="3:12" customFormat="1" ht="14.75" customHeight="1">
       <c r="E11" s="50"/>
@@ -7221,7 +7316,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -7246,7 +7341,7 @@
         <v>208</v>
       </c>
       <c r="H3" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:8">

</xml_diff>

<commit_message>
update files ca nomenclature
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966DCB2E-8B95-3548-A00F-6C32B028A003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2583AD-FA70-3E46-9D27-EA4B944025EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="S0xIUhd+qm/mil3mjEDLzBXqSnUj+E9UJlwfUt2w9pzFPXpGrV21CR6+VbcA2GUl+o5ORpHAcx1Tl5P1yPCQ/w==" workbookSaltValue="Ic6K1fVcoeoWgJU+jzPQ6w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19200" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille de temps" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="364">
   <si>
     <t>Temps de travail d'un magistrat</t>
   </si>
@@ -565,9 +565,6 @@
     <t>1.4.</t>
   </si>
   <si>
-    <t>AUTRES CONTENTIEUX SOCIAUX</t>
-  </si>
-  <si>
     <t>1.</t>
   </si>
   <si>
@@ -595,9 +592,6 @@
     <t>2.7.</t>
   </si>
   <si>
-    <t>TUTELLES MINEURS</t>
-  </si>
-  <si>
     <t>2.8.</t>
   </si>
   <si>
@@ -610,24 +604,12 @@
     <t>3.2.</t>
   </si>
   <si>
-    <t>PROTECTION DES MAJEURS</t>
-  </si>
-  <si>
     <t>3.3.</t>
   </si>
   <si>
-    <t>BAUX</t>
-  </si>
-  <si>
-    <t>CRÉDIT À LA CONSOMMATION</t>
-  </si>
-  <si>
     <t>3.5.</t>
   </si>
   <si>
-    <t>AUTRES CONTENTIEUX DE LA PROTECTION</t>
-  </si>
-  <si>
     <t>3.</t>
   </si>
   <si>
@@ -646,27 +628,12 @@
     <t>4.4.</t>
   </si>
   <si>
-    <t>RESPONSABILITÉ ET QUASI-CONTRATS</t>
-  </si>
-  <si>
     <t>4.5.</t>
   </si>
   <si>
-    <t>DROIT DES BIENS</t>
-  </si>
-  <si>
     <t>4.6.</t>
   </si>
   <si>
-    <t>CONSTRUCTION</t>
-  </si>
-  <si>
-    <t>DROIT DES AFFAIRES</t>
-  </si>
-  <si>
-    <t>INTÉRÊTS CIVILS</t>
-  </si>
-  <si>
     <t>CIVI</t>
   </si>
   <si>
@@ -679,39 +646,21 @@
     <t>5.1.</t>
   </si>
   <si>
-    <t>JLD CIVIL</t>
-  </si>
-  <si>
     <t>5.2.</t>
   </si>
   <si>
     <t>5.3.</t>
   </si>
   <si>
-    <t>AUTRES JLD CIVIL</t>
-  </si>
-  <si>
     <t>5.</t>
   </si>
   <si>
-    <t>TOTAL JLD CIVIL</t>
-  </si>
-  <si>
-    <t>6.1.</t>
-  </si>
-  <si>
     <t>ACTIVITÉ CIVILE</t>
   </si>
   <si>
-    <t>6.2.</t>
-  </si>
-  <si>
     <t>ACTIVITÉ PÉNALE</t>
   </si>
   <si>
-    <t>6.</t>
-  </si>
-  <si>
     <t>7.1.</t>
   </si>
   <si>
@@ -766,21 +715,9 @@
     <t>AUTRES ACTIVITÉS</t>
   </si>
   <si>
-    <t>SOUTIEN (HORS FORMATIONS SUIVIES)</t>
-  </si>
-  <si>
-    <t>FORMATIONS SUIVIES</t>
-  </si>
-  <si>
     <t>11.3.</t>
   </si>
   <si>
-    <t>FORMATIONS DISPENSÉES</t>
-  </si>
-  <si>
-    <t>ACCÈS AU DROIT ET À LA JUSTICE</t>
-  </si>
-  <si>
     <t>CSM</t>
   </si>
   <si>
@@ -1021,45 +958,12 @@
     <t>JP</t>
   </si>
   <si>
-    <t>CONTENTIEUX DU TRAVAIL</t>
-  </si>
-  <si>
-    <t>PROTECTION SOCIALE</t>
-  </si>
-  <si>
-    <t>APPEL DES RÉFÉRÉS CPH</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>COMMERCIAL</t>
   </si>
   <si>
-    <t>CONTENTIEUX COMMERCIAL GÉNÉRAL</t>
-  </si>
-  <si>
-    <t>PROCÉDURES COLLECTIVES</t>
-  </si>
-  <si>
-    <t>DROIT DES SOCIÉTÉS</t>
-  </si>
-  <si>
-    <t>CONCURRENCE</t>
-  </si>
-  <si>
-    <t>BAUX COMMERCIAUX</t>
-  </si>
-  <si>
-    <t>PROPRIÉTÉ INTELLECTUELLE ET INDUSTRIELLE</t>
-  </si>
-  <si>
-    <t>RECOURS SPÉCIFIQUES</t>
-  </si>
-  <si>
-    <t>AUTRES CONTENTIEUX COMMERCIAUX</t>
-  </si>
-  <si>
     <t>TOTAL COMMERCIAL</t>
   </si>
   <si>
@@ -1069,60 +973,27 @@
     <t>FAMILLE</t>
   </si>
   <si>
-    <t>CONTENTIEUX GÉNÉRAL DE LA FAMILLE</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX PATRIMONIAL DE LA FAMILLE</t>
-  </si>
-  <si>
-    <t>ETAT DES PERSONNES</t>
-  </si>
-  <si>
-    <t>3.4.</t>
-  </si>
-  <si>
-    <t>AUTRES CONTENTIEUX DE LA FAMILLE</t>
-  </si>
-  <si>
     <t>TOTAL FAMILLE</t>
   </si>
   <si>
     <t>PROTECTION</t>
   </si>
   <si>
-    <t>SURENDETTEMENT</t>
-  </si>
-  <si>
-    <t>APPEL DES RÉFÉRÉS DU JCP</t>
-  </si>
-  <si>
     <t>TOTAL PROTECTION</t>
   </si>
   <si>
     <t>5.4.</t>
   </si>
   <si>
-    <t>CONTENTIEUX CONTRACTUEL</t>
-  </si>
-  <si>
     <t>5.5.</t>
   </si>
   <si>
-    <t>EXPROPRIATION</t>
-  </si>
-  <si>
     <t>5.6.</t>
   </si>
   <si>
-    <t>SÛRETÉS ET EXÉCUTION</t>
-  </si>
-  <si>
     <t>5.7.</t>
   </si>
   <si>
-    <t>APPEL DES RÉFÉRÉS CIVILS</t>
-  </si>
-  <si>
     <t>5.8.</t>
   </si>
   <si>
@@ -1132,51 +1003,15 @@
     <t>5.10.</t>
   </si>
   <si>
-    <t>AUTRES CONTENTIEUX CIVILS NS</t>
-  </si>
-  <si>
-    <t>DROIT DES ÉTRANGERS</t>
-  </si>
-  <si>
-    <t>HO - CONTENTION</t>
-  </si>
-  <si>
-    <t>6.3.</t>
-  </si>
-  <si>
-    <t>VISITES DOMICILIAIRES</t>
-  </si>
-  <si>
-    <t>6.4.</t>
-  </si>
-  <si>
     <t>MINEURS</t>
   </si>
   <si>
     <t>TOTAL MINEURS</t>
   </si>
   <si>
-    <t>CORRECTIONNEL</t>
-  </si>
-  <si>
-    <t>POUVOIRS PROPRES DU PRÉSIDENT</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX GÉNÉRAL HORS JIRS</t>
-  </si>
-  <si>
-    <t>ECO-FI ET CRIM-ORG HORS JIRS</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX JIRS</t>
-  </si>
-  <si>
     <t>8.5.</t>
   </si>
   <si>
-    <t>CONTENTIEUX DU TRIBUNAL DE POLICE</t>
-  </si>
-  <si>
     <t>8.6.</t>
   </si>
   <si>
@@ -1186,114 +1021,45 @@
     <t>INSTRUCTION ET ENTRAIDE</t>
   </si>
   <si>
-    <t>CONTENTIEUX DE LA DÉTENTION HORS JIRS</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX DE LA DÉTENTION JIRS</t>
-  </si>
-  <si>
-    <t>CONTENTIEUX DU CONTRÔLE JUDICIAIRE HORS JIRS</t>
-  </si>
-  <si>
     <t>9.5.</t>
   </si>
   <si>
-    <t>CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS</t>
-  </si>
-  <si>
     <t>9.6.</t>
   </si>
   <si>
-    <t>CONTENTIEUX DE FOND HORS JIRS</t>
-  </si>
-  <si>
     <t>9.7.</t>
   </si>
   <si>
-    <t>CONTENTIEUX DE FOND JIRS</t>
-  </si>
-  <si>
     <t>9.8.</t>
   </si>
   <si>
-    <t>ENTRAIDE PÉNALE</t>
-  </si>
-  <si>
     <t>9.9</t>
   </si>
   <si>
-    <t>CONTENTIEUX DE FOND AUTRES CONTENTIEUX SPÉCIALISÉS</t>
-  </si>
-  <si>
     <t>TOTAL INSTRUCTION ET ENTRAIDE</t>
   </si>
   <si>
     <t>APPLICATION DES PEINES</t>
   </si>
   <si>
-    <t>CHAMBRE DE L'APPLICATION DES PEINES</t>
-  </si>
-  <si>
     <t>10.3.</t>
   </si>
   <si>
-    <t>TRIBUNAL DE L'APPLICATION DES PEINES</t>
-  </si>
-  <si>
     <t>10.4.</t>
   </si>
   <si>
-    <t>JURIDICTION RÉGIONALE DES MESURES DE SÛRETÉ</t>
-  </si>
-  <si>
     <t>TOTAL APPLICATION DES PEINES</t>
   </si>
   <si>
     <t>CRIMINEL</t>
   </si>
   <si>
-    <t>ASSISES HORS JIRS</t>
-  </si>
-  <si>
     <t>11.2</t>
   </si>
   <si>
-    <t>ASSISES JIRS</t>
-  </si>
-  <si>
-    <t>COUR CRIMINELLE DÉPARTEMENTALE</t>
-  </si>
-  <si>
     <t>TOTAL CRIMINEL</t>
   </si>
   <si>
-    <t>12.1.</t>
-  </si>
-  <si>
-    <t>CONTESTATION DES HONORAIRES</t>
-  </si>
-  <si>
-    <t>12.2.</t>
-  </si>
-  <si>
-    <t>INDEMNISATION DE LA DP</t>
-  </si>
-  <si>
-    <t>12.3.</t>
-  </si>
-  <si>
-    <t>RÉFÉRÉS PP</t>
-  </si>
-  <si>
-    <t>12.4.</t>
-  </si>
-  <si>
-    <t>AUTRES ATTRIBUTIONS DU PP</t>
-  </si>
-  <si>
-    <t>12.</t>
-  </si>
-  <si>
     <t>13.1.</t>
   </si>
   <si>
@@ -1309,40 +1075,298 @@
     <t>13.5.</t>
   </si>
   <si>
-    <t>EXPERTISES (SUIVI ET LISTES)</t>
-  </si>
-  <si>
     <t>13.6.</t>
   </si>
   <si>
-    <t>MÉDIATION (SUIVI ET LISTES)</t>
-  </si>
-  <si>
     <t>13.7.</t>
   </si>
   <si>
     <t>13.8.</t>
   </si>
   <si>
-    <t>ACCUEIL DU JUSTICIABLE</t>
-  </si>
-  <si>
     <t>13.9.</t>
   </si>
   <si>
-    <t>FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL</t>
-  </si>
-  <si>
     <t>13.10.</t>
   </si>
   <si>
-    <t>AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL</t>
-  </si>
-  <si>
     <t>13.</t>
   </si>
   <si>
     <t>TOTAL PP</t>
+  </si>
+  <si>
+    <t>Contentieux du travail</t>
+  </si>
+  <si>
+    <t>Protection sociale</t>
+  </si>
+  <si>
+    <t>Appel des référés CPH</t>
+  </si>
+  <si>
+    <t>Autres contentieux sociaux</t>
+  </si>
+  <si>
+    <t>Contentieux commercial général</t>
+  </si>
+  <si>
+    <t>Procédures collectives</t>
+  </si>
+  <si>
+    <t>Droit des affaires</t>
+  </si>
+  <si>
+    <t>Droit des sociétés</t>
+  </si>
+  <si>
+    <t>Concurrence</t>
+  </si>
+  <si>
+    <t>Baux commerciaux</t>
+  </si>
+  <si>
+    <t>Propriété intellectuelle et industrielle</t>
+  </si>
+  <si>
+    <t>Recours spécifiques</t>
+  </si>
+  <si>
+    <t>Autres contentieux commerciaux</t>
+  </si>
+  <si>
+    <t>Contentieux général de la famille</t>
+  </si>
+  <si>
+    <t>Contentieux patrimonial de la famille</t>
+  </si>
+  <si>
+    <t>Etat des personnes</t>
+  </si>
+  <si>
+    <t>Autres contentieux de la famille</t>
+  </si>
+  <si>
+    <t>Protection des majeurs</t>
+  </si>
+  <si>
+    <t>Baux</t>
+  </si>
+  <si>
+    <t>Surendettement</t>
+  </si>
+  <si>
+    <t>Crédit à la consommation</t>
+  </si>
+  <si>
+    <t>Appel des référés du JCP</t>
+  </si>
+  <si>
+    <t>Autres contentieux de la protection</t>
+  </si>
+  <si>
+    <t>Tutelles mineurs</t>
+  </si>
+  <si>
+    <t>4.7.</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Autres contentieux civils NS</t>
+  </si>
+  <si>
+    <t>Droit des biens</t>
+  </si>
+  <si>
+    <t>Responsabilité et quasi-contrats</t>
+  </si>
+  <si>
+    <t>Contentieux contractuel</t>
+  </si>
+  <si>
+    <t>Expropriation</t>
+  </si>
+  <si>
+    <t>Sûretés et exécution</t>
+  </si>
+  <si>
+    <t>Appel des référés civils</t>
+  </si>
+  <si>
+    <t>Pouvoirs propres du Président</t>
+  </si>
+  <si>
+    <t>Contentieux collégial hors JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux spécialisés hors JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux JIRS crim-org</t>
+  </si>
+  <si>
+    <t>Contentieux du tribunal de Police</t>
+  </si>
+  <si>
+    <t>Intérêts civils</t>
+  </si>
+  <si>
+    <t>Contentieux JIRS éco-fi</t>
+  </si>
+  <si>
+    <t>Autres correctionnel</t>
+  </si>
+  <si>
+    <t>Contentieux à conseiller unique</t>
+  </si>
+  <si>
+    <t>8.7.</t>
+  </si>
+  <si>
+    <t>8.8.</t>
+  </si>
+  <si>
+    <t>8.9.</t>
+  </si>
+  <si>
+    <t>Autres CHINS</t>
+  </si>
+  <si>
+    <t>Contentieux de la détention hors JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux de la détention JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux de fond hors JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux de fond JIRS</t>
+  </si>
+  <si>
+    <t>Entraide pénale</t>
+  </si>
+  <si>
+    <t>Contentieux de fond contentieux spécialisés</t>
+  </si>
+  <si>
+    <t>Contentieux du contrôle judiciaire JIRS</t>
+  </si>
+  <si>
+    <t>Contentieux du contrôle judiciaire hors JIRS</t>
+  </si>
+  <si>
+    <t>9.10.</t>
+  </si>
+  <si>
+    <t>Appels TAP</t>
+  </si>
+  <si>
+    <t>Juridiction régionale de la rétention de sûreté</t>
+  </si>
+  <si>
+    <t>Autres CHAP</t>
+  </si>
+  <si>
+    <t>Assises hors JIRS</t>
+  </si>
+  <si>
+    <t>Assises JIRS</t>
+  </si>
+  <si>
+    <t>Cour criminelle départementale</t>
+  </si>
+  <si>
+    <t>Contestation des honoraires, frais et dépens</t>
+  </si>
+  <si>
+    <t>Indemnisation de la DP</t>
+  </si>
+  <si>
+    <t>Procédures urgentes</t>
+  </si>
+  <si>
+    <t>Autres attributions du PP</t>
+  </si>
+  <si>
+    <t>Extraditions et MAE</t>
+  </si>
+  <si>
+    <t>Saisies et confiscations des avoirs criminels</t>
+  </si>
+  <si>
+    <t>Droit des étrangers</t>
+  </si>
+  <si>
+    <t>HO - Contention</t>
+  </si>
+  <si>
+    <t>Autres appels JLD</t>
+  </si>
+  <si>
+    <t>Soutien (autres)</t>
+  </si>
+  <si>
+    <t>Autres fonctionnaires / JA affectés au parquet général</t>
+  </si>
+  <si>
+    <t>Activités extérieures et partenariats</t>
+  </si>
+  <si>
+    <t>Équipement</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Politique associative et aide aux victimes</t>
+  </si>
+  <si>
+    <t>Autres activités non juridictionnelles</t>
+  </si>
+  <si>
+    <t>Formations suivies</t>
+  </si>
+  <si>
+    <t>Formations dispensées</t>
+  </si>
+  <si>
+    <t>Expertises (suivi et listes)</t>
+  </si>
+  <si>
+    <t>Médiation / conciliation (suivi et listes)</t>
+  </si>
+  <si>
+    <t>Accès au droit et à la Justice</t>
+  </si>
+  <si>
+    <t>Accueil du justiciable</t>
+  </si>
+  <si>
+    <t>Fonctionnaires / JA affectés aux activités civiles et commerciales du parquet général</t>
+  </si>
+  <si>
+    <t>13.11.</t>
+  </si>
+  <si>
+    <t>13.12.</t>
+  </si>
+  <si>
+    <t>13.13.</t>
+  </si>
+  <si>
+    <t>13.14.</t>
+  </si>
+  <si>
+    <t>13.15.</t>
+  </si>
+  <si>
+    <t>10.5.</t>
+  </si>
+  <si>
+    <t>Appels JAP</t>
   </si>
 </sst>
 </file>
@@ -1357,7 +1381,7 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1536,12 +1560,6 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1727,7 +1745,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2127,17 +2145,10 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2155,6 +2166,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2209,6 +2223,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4176,7 +4193,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE60DF7-F7D7-42C7-82AA-8FB5759BD1A1}">
   <sheetPr codeName="Feuil4"/>
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -4244,12 +4261,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="121"/>
-      <c r="B6" s="146" t="s">
+      <c r="B6" s="143" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="147"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="144"/>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
@@ -4264,7 +4281,7 @@
         <v>88</v>
       </c>
       <c r="E7" s="129">
-        <f>SUM(E13,E23,E29,E36,E47,E52,E55,E62,E72,E77,E81,E86,E97)/100</f>
+        <f>SUM(E13,E23,E28,E36,E47,E60,E70,E81,E87,E91,E57,E107)/100</f>
         <v>0</v>
       </c>
       <c r="F7" s="42"/>
@@ -4274,8 +4291,8 @@
       <c r="B8" s="130" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="148"/>
-      <c r="D8" s="149"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="131" t="s">
         <v>90</v>
       </c>
@@ -4285,11 +4302,11 @@
       <c r="A9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="142" t="s">
+      <c r="B9" s="140" t="s">
         <v>92</v>
       </c>
       <c r="C9" s="132" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="D9" s="132"/>
       <c r="E9" s="133"/>
@@ -4299,9 +4316,9 @@
       <c r="A10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="144"/>
+      <c r="B10" s="147"/>
       <c r="C10" s="132" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="D10" s="132"/>
       <c r="E10" s="133"/>
@@ -4311,9 +4328,9 @@
       <c r="A11" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="144"/>
+      <c r="B11" s="147"/>
       <c r="C11" s="132" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="D11" s="132"/>
       <c r="E11" s="133"/>
@@ -4323,9 +4340,9 @@
       <c r="A12" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="144"/>
+      <c r="B12" s="147"/>
       <c r="C12" s="132" t="s">
-        <v>96</v>
+        <v>276</v>
       </c>
       <c r="D12" s="132"/>
       <c r="E12" s="133"/>
@@ -4333,16 +4350,16 @@
     </row>
     <row r="13" spans="1:7" ht="28" customHeight="1" thickBot="1">
       <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="134" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="134" t="s">
-        <v>98</v>
-      </c>
       <c r="C13" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D13" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E13" s="136">
         <f>SUM(E9:E12)</f>
@@ -4352,13 +4369,13 @@
     </row>
     <row r="14" spans="1:7" ht="16" thickTop="1">
       <c r="A14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="142" t="s">
-        <v>252</v>
+        <v>98</v>
+      </c>
+      <c r="B14" s="140" t="s">
+        <v>228</v>
       </c>
       <c r="C14" s="132" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="D14" s="132"/>
       <c r="E14" s="133"/>
@@ -4366,11 +4383,11 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="144"/>
+        <v>101</v>
+      </c>
+      <c r="B15" s="166"/>
       <c r="C15" s="132" t="s">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="D15" s="132"/>
       <c r="E15" s="133"/>
@@ -4378,11 +4395,11 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="144"/>
+        <v>99</v>
+      </c>
+      <c r="B16" s="147"/>
       <c r="C16" s="132" t="s">
-        <v>128</v>
+        <v>278</v>
       </c>
       <c r="D16" s="132"/>
       <c r="E16" s="133"/>
@@ -4390,11 +4407,11 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="144"/>
+        <v>103</v>
+      </c>
+      <c r="B17" s="147"/>
       <c r="C17" s="132" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="D17" s="132"/>
       <c r="E17" s="133"/>
@@ -4402,11 +4419,11 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="145"/>
+        <v>100</v>
+      </c>
+      <c r="B18" s="147"/>
       <c r="C18" s="132" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
       <c r="D18" s="132"/>
       <c r="E18" s="133"/>
@@ -4416,9 +4433,9 @@
       <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="145"/>
+      <c r="B19" s="142"/>
       <c r="C19" s="132" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="D19" s="132"/>
       <c r="E19" s="133"/>
@@ -4426,11 +4443,11 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="145"/>
+        <v>102</v>
+      </c>
+      <c r="B20" s="142"/>
       <c r="C20" s="132" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="D20" s="132"/>
       <c r="E20" s="133"/>
@@ -4438,11 +4455,11 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="145"/>
+        <v>105</v>
+      </c>
+      <c r="B21" s="142"/>
       <c r="C21" s="132" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="D21" s="132"/>
       <c r="E21" s="133"/>
@@ -4450,11 +4467,11 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="145"/>
+        <v>106</v>
+      </c>
+      <c r="B22" s="142"/>
       <c r="C22" s="132" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
       <c r="D22" s="132"/>
       <c r="E22" s="133"/>
@@ -4462,16 +4479,16 @@
     </row>
     <row r="23" spans="1:6" ht="38" customHeight="1" thickBot="1">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B23" s="134" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="C23" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D23" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E23" s="136">
         <f>SUM(E14:E22)</f>
@@ -4481,13 +4498,13 @@
     </row>
     <row r="24" spans="1:6" ht="16" thickTop="1">
       <c r="A24" t="s">
-        <v>262</v>
-      </c>
-      <c r="B24" s="142" t="s">
-        <v>263</v>
+        <v>230</v>
+      </c>
+      <c r="B24" s="140" t="s">
+        <v>231</v>
       </c>
       <c r="C24" s="132" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="D24" s="132"/>
       <c r="E24" s="133"/>
@@ -4495,11 +4512,11 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="144"/>
+        <v>108</v>
+      </c>
+      <c r="B25" s="147"/>
       <c r="C25" s="132" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="D25" s="132"/>
       <c r="E25" s="133"/>
@@ -4507,11 +4524,11 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" s="144"/>
+        <v>109</v>
+      </c>
+      <c r="B26" s="147"/>
       <c r="C26" s="132" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="D26" s="132"/>
       <c r="E26" s="133"/>
@@ -4519,56 +4536,56 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>267</v>
-      </c>
-      <c r="B27" s="144"/>
+        <v>110</v>
+      </c>
+      <c r="B27" s="147"/>
       <c r="C27" s="132" t="s">
-        <v>106</v>
+        <v>289</v>
       </c>
       <c r="D27" s="132"/>
       <c r="E27" s="133"/>
       <c r="F27" s="42"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="16" thickBot="1">
       <c r="A28" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28" s="145"/>
-      <c r="C28" s="132" t="s">
-        <v>268</v>
-      </c>
-      <c r="D28" s="132"/>
-      <c r="E28" s="133"/>
+        <v>111</v>
+      </c>
+      <c r="B28" s="134" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D28" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E28" s="136">
+        <f>SUM(E24:E27)</f>
+        <v>0</v>
+      </c>
       <c r="F28" s="42"/>
     </row>
-    <row r="29" spans="1:6" ht="16" thickBot="1">
+    <row r="29" spans="1:6" ht="16" thickTop="1">
       <c r="A29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="134" t="s">
-        <v>269</v>
-      </c>
-      <c r="C29" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D29" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E29" s="136">
-        <f>SUM(E24:E28)</f>
-        <v>0</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B29" s="140" t="s">
+        <v>233</v>
+      </c>
+      <c r="C29" s="132" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="132"/>
+      <c r="E29" s="133"/>
       <c r="F29" s="42"/>
     </row>
-    <row r="30" spans="1:6" ht="16" thickTop="1">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>119</v>
-      </c>
-      <c r="B30" s="142" t="s">
-        <v>270</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="B30" s="147"/>
       <c r="C30" s="132" t="s">
-        <v>111</v>
+        <v>296</v>
       </c>
       <c r="D30" s="132"/>
       <c r="E30" s="133"/>
@@ -4576,11 +4593,11 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>120</v>
-      </c>
-      <c r="B31" s="144"/>
+        <v>115</v>
+      </c>
+      <c r="B31" s="147"/>
       <c r="C31" s="132" t="s">
-        <v>113</v>
+        <v>292</v>
       </c>
       <c r="D31" s="132"/>
       <c r="E31" s="133"/>
@@ -4588,11 +4605,11 @@
     </row>
     <row r="32" spans="1:6" ht="26" customHeight="1">
       <c r="A32" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="144"/>
+        <v>116</v>
+      </c>
+      <c r="B32" s="147"/>
       <c r="C32" s="132" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="D32" s="132"/>
       <c r="E32" s="133"/>
@@ -4600,11 +4617,11 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B33" s="144"/>
+        <v>114</v>
+      </c>
+      <c r="B33" s="147"/>
       <c r="C33" s="132" t="s">
-        <v>114</v>
+        <v>291</v>
       </c>
       <c r="D33" s="132"/>
       <c r="E33" s="133"/>
@@ -4612,11 +4629,11 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="145"/>
+        <v>117</v>
+      </c>
+      <c r="B34" s="142"/>
       <c r="C34" s="132" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="D34" s="132"/>
       <c r="E34" s="133"/>
@@ -4624,11 +4641,11 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" s="145"/>
+        <v>118</v>
+      </c>
+      <c r="B35" s="142"/>
       <c r="C35" s="132" t="s">
-        <v>116</v>
+        <v>295</v>
       </c>
       <c r="D35" s="132"/>
       <c r="E35" s="133"/>
@@ -4636,32 +4653,32 @@
     </row>
     <row r="36" spans="1:6" ht="16" thickBot="1">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B36" s="134" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="C36" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D36" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E36" s="136">
-        <f>SUM(E30:E35)</f>
+        <f>SUM(E29:E35)</f>
         <v>0</v>
       </c>
       <c r="F36" s="42"/>
     </row>
     <row r="37" spans="1:6" ht="16" thickTop="1">
       <c r="A37" t="s">
-        <v>133</v>
-      </c>
-      <c r="B37" s="142" t="s">
-        <v>118</v>
+        <v>235</v>
+      </c>
+      <c r="B37" s="140" t="s">
+        <v>112</v>
       </c>
       <c r="C37" s="132" t="s">
-        <v>127</v>
+        <v>302</v>
       </c>
       <c r="D37" s="132"/>
       <c r="E37" s="133"/>
@@ -4669,11 +4686,11 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B38" s="144"/>
+        <v>124</v>
+      </c>
+      <c r="B38" s="147"/>
       <c r="C38" s="132" t="s">
-        <v>125</v>
+        <v>301</v>
       </c>
       <c r="D38" s="132"/>
       <c r="E38" s="133"/>
@@ -4681,11 +4698,11 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" s="144"/>
+        <v>123</v>
+      </c>
+      <c r="B39" s="147"/>
       <c r="C39" s="132" t="s">
-        <v>123</v>
+        <v>300</v>
       </c>
       <c r="D39" s="132"/>
       <c r="E39" s="133"/>
@@ -4693,11 +4710,11 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B40" s="145"/>
+        <v>122</v>
+      </c>
+      <c r="B40" s="147"/>
       <c r="C40" s="132" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="D40" s="132"/>
       <c r="E40" s="133"/>
@@ -4705,11 +4722,11 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>276</v>
-      </c>
-      <c r="B41" s="145"/>
+        <v>237</v>
+      </c>
+      <c r="B41" s="147"/>
       <c r="C41" s="132" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="D41" s="132"/>
       <c r="E41" s="133"/>
@@ -4717,11 +4734,11 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>278</v>
-      </c>
-      <c r="B42" s="145"/>
+        <v>236</v>
+      </c>
+      <c r="B42" s="142"/>
       <c r="C42" s="132" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="D42" s="132"/>
       <c r="E42" s="133"/>
@@ -4729,11 +4746,11 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>280</v>
-      </c>
-      <c r="B43" s="145"/>
+        <v>238</v>
+      </c>
+      <c r="B43" s="142"/>
       <c r="C43" s="132" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="D43" s="132"/>
       <c r="E43" s="133"/>
@@ -4741,11 +4758,11 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>282</v>
-      </c>
-      <c r="B44" s="145"/>
+        <v>239</v>
+      </c>
+      <c r="B44" s="142"/>
       <c r="C44" s="132" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D44" s="132"/>
       <c r="E44" s="133"/>
@@ -4753,11 +4770,11 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>283</v>
-      </c>
-      <c r="B45" s="145"/>
+        <v>240</v>
+      </c>
+      <c r="B45" s="142"/>
       <c r="C45" s="132" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="D45" s="132"/>
       <c r="E45" s="133"/>
@@ -4765,11 +4782,11 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>284</v>
-      </c>
-      <c r="B46" s="145"/>
+        <v>241</v>
+      </c>
+      <c r="B46" s="142"/>
       <c r="C46" s="132" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="D46" s="132"/>
       <c r="E46" s="133"/>
@@ -4777,16 +4794,16 @@
     </row>
     <row r="47" spans="1:6" ht="16" thickBot="1">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B47" s="134" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C47" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D47" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E47" s="136">
         <f>SUM(E37:E46)</f>
@@ -4795,152 +4812,113 @@
       <c r="F47" s="42"/>
     </row>
     <row r="48" spans="1:6" ht="16" thickTop="1">
-      <c r="A48" t="s">
-        <v>140</v>
-      </c>
-      <c r="B48" s="142" t="s">
-        <v>134</v>
+      <c r="B48" s="140" t="s">
+        <v>204</v>
       </c>
       <c r="C48" s="132" t="s">
-        <v>286</v>
+        <v>334</v>
       </c>
       <c r="D48" s="132"/>
       <c r="E48" s="133"/>
       <c r="F48" s="42"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>142</v>
-      </c>
-      <c r="B49" s="144"/>
+      <c r="B49" s="166"/>
       <c r="C49" s="132" t="s">
-        <v>287</v>
+        <v>335</v>
       </c>
       <c r="D49" s="132"/>
       <c r="E49" s="133"/>
       <c r="F49" s="42"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>288</v>
-      </c>
-      <c r="B50" s="144"/>
+      <c r="B50" s="166"/>
       <c r="C50" s="132" t="s">
-        <v>289</v>
+        <v>336</v>
       </c>
       <c r="D50" s="132"/>
       <c r="E50" s="133"/>
       <c r="F50" s="42"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>290</v>
-      </c>
-      <c r="B51" s="144"/>
+      <c r="B51" s="166"/>
       <c r="C51" s="132" t="s">
-        <v>137</v>
+        <v>337</v>
       </c>
       <c r="D51" s="132"/>
       <c r="E51" s="133"/>
       <c r="F51" s="42"/>
     </row>
-    <row r="52" spans="1:6" ht="33" customHeight="1" thickBot="1">
-      <c r="A52" t="s">
-        <v>144</v>
-      </c>
-      <c r="B52" s="134" t="s">
-        <v>139</v>
-      </c>
-      <c r="C52" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D52" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E52" s="136">
-        <f>SUM(E48:E51)</f>
-        <v>0</v>
-      </c>
+    <row r="52" spans="1:6">
+      <c r="B52" s="166"/>
+      <c r="C52" s="132" t="s">
+        <v>338</v>
+      </c>
+      <c r="D52" s="132"/>
+      <c r="E52" s="133"/>
       <c r="F52" s="42"/>
     </row>
-    <row r="53" spans="1:6" ht="16" thickTop="1">
-      <c r="A53" t="s">
-        <v>145</v>
-      </c>
-      <c r="B53" s="142" t="s">
-        <v>291</v>
-      </c>
+    <row r="53" spans="1:6">
+      <c r="B53" s="141"/>
       <c r="C53" s="132" t="s">
-        <v>141</v>
+        <v>339</v>
       </c>
       <c r="D53" s="132"/>
       <c r="E53" s="133"/>
       <c r="F53" s="42"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>146</v>
-      </c>
-      <c r="B54" s="143"/>
+      <c r="B54" s="141"/>
       <c r="C54" s="132" t="s">
-        <v>143</v>
+        <v>340</v>
       </c>
       <c r="D54" s="132"/>
       <c r="E54" s="133"/>
       <c r="F54" s="42"/>
     </row>
-    <row r="55" spans="1:6" ht="16" thickBot="1">
-      <c r="A55" t="s">
-        <v>147</v>
-      </c>
-      <c r="B55" s="134" t="s">
-        <v>292</v>
-      </c>
-      <c r="C55" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D55" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E55" s="136">
-        <f>SUM(E53:E54)</f>
-        <v>0</v>
-      </c>
+    <row r="55" spans="1:6">
+      <c r="B55" s="141"/>
+      <c r="C55" s="132" t="s">
+        <v>341</v>
+      </c>
+      <c r="D55" s="132"/>
+      <c r="E55" s="133"/>
       <c r="F55" s="42"/>
     </row>
-    <row r="56" spans="1:6" ht="16" thickTop="1">
-      <c r="A56" t="s">
-        <v>148</v>
-      </c>
-      <c r="B56" s="142" t="s">
-        <v>293</v>
-      </c>
+    <row r="56" spans="1:6">
+      <c r="B56" s="142"/>
       <c r="C56" s="132" t="s">
-        <v>294</v>
+        <v>342</v>
       </c>
       <c r="D56" s="132"/>
       <c r="E56" s="133"/>
       <c r="F56" s="42"/>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>149</v>
-      </c>
-      <c r="B57" s="144"/>
-      <c r="C57" s="132" t="s">
-        <v>295</v>
-      </c>
-      <c r="D57" s="132"/>
-      <c r="E57" s="133"/>
+    <row r="57" spans="1:6" ht="16" thickBot="1">
+      <c r="B57" s="134" t="s">
+        <v>272</v>
+      </c>
+      <c r="C57" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D57" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E57" s="136">
+        <f>SUM(E48:E56)</f>
+        <v>0</v>
+      </c>
       <c r="F57" s="42"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" ht="16" thickTop="1">
       <c r="A58" t="s">
-        <v>150</v>
-      </c>
-      <c r="B58" s="144"/>
+        <v>128</v>
+      </c>
+      <c r="B58" s="140" t="s">
+        <v>242</v>
+      </c>
       <c r="C58" s="132" t="s">
-        <v>296</v>
+        <v>126</v>
       </c>
       <c r="D58" s="132"/>
       <c r="E58" s="133"/>
@@ -4948,68 +4926,66 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>151</v>
-      </c>
-      <c r="B59" s="144"/>
+        <v>129</v>
+      </c>
+      <c r="B59" s="141"/>
       <c r="C59" s="132" t="s">
-        <v>297</v>
+        <v>127</v>
       </c>
       <c r="D59" s="132"/>
       <c r="E59" s="133"/>
       <c r="F59" s="42"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" ht="16" thickBot="1">
       <c r="A60" t="s">
-        <v>298</v>
-      </c>
-      <c r="B60" s="145"/>
-      <c r="C60" s="132" t="s">
-        <v>299</v>
-      </c>
-      <c r="D60" s="132"/>
-      <c r="E60" s="133"/>
+        <v>130</v>
+      </c>
+      <c r="B60" s="134" t="s">
+        <v>243</v>
+      </c>
+      <c r="C60" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D60" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E60" s="136">
+        <f>SUM(E58:E59)</f>
+        <v>0</v>
+      </c>
       <c r="F60" s="42"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" ht="16" thickTop="1">
       <c r="A61" t="s">
-        <v>300</v>
-      </c>
-      <c r="B61" s="145"/>
+        <v>131</v>
+      </c>
+      <c r="B61" s="166"/>
       <c r="C61" s="132" t="s">
-        <v>129</v>
+        <v>306</v>
       </c>
       <c r="D61" s="132"/>
       <c r="E61" s="133"/>
       <c r="F61" s="42"/>
     </row>
-    <row r="62" spans="1:6" ht="16" thickBot="1">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>152</v>
-      </c>
-      <c r="B62" s="134" t="s">
-        <v>301</v>
-      </c>
-      <c r="C62" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D62" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E62" s="136">
-        <f>SUM(E56:E61)</f>
-        <v>0</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="B62" s="147"/>
+      <c r="C62" s="132" t="s">
+        <v>307</v>
+      </c>
+      <c r="D62" s="132"/>
+      <c r="E62" s="133"/>
       <c r="F62" s="42"/>
     </row>
-    <row r="63" spans="1:6" ht="16" thickTop="1">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>153</v>
-      </c>
-      <c r="B63" s="142" t="s">
-        <v>302</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="B63" s="147"/>
       <c r="C63" s="132" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="D63" s="132"/>
       <c r="E63" s="133"/>
@@ -5017,11 +4993,11 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>154</v>
-      </c>
-      <c r="B64" s="144"/>
+        <v>134</v>
+      </c>
+      <c r="B64" s="147"/>
       <c r="C64" s="132" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="D64" s="132"/>
       <c r="E64" s="133"/>
@@ -5029,11 +5005,11 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>155</v>
-      </c>
-      <c r="B65" s="144"/>
+        <v>315</v>
+      </c>
+      <c r="B65" s="147"/>
       <c r="C65" s="132" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="D65" s="132"/>
       <c r="E65" s="133"/>
@@ -5041,11 +5017,11 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>156</v>
-      </c>
-      <c r="B66" s="144"/>
+        <v>317</v>
+      </c>
+      <c r="B66" s="147"/>
       <c r="C66" s="132" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="D66" s="132"/>
       <c r="E66" s="133"/>
@@ -5053,11 +5029,11 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>306</v>
-      </c>
-      <c r="B67" s="145"/>
+        <v>244</v>
+      </c>
+      <c r="B67" s="142"/>
       <c r="C67" s="132" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D67" s="132"/>
       <c r="E67" s="133"/>
@@ -5065,11 +5041,11 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>308</v>
-      </c>
-      <c r="B68" s="145"/>
+        <v>245</v>
+      </c>
+      <c r="B68" s="142"/>
       <c r="C68" s="132" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D68" s="132"/>
       <c r="E68" s="133"/>
@@ -5077,68 +5053,68 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>310</v>
-      </c>
-      <c r="B69" s="145"/>
+        <v>316</v>
+      </c>
+      <c r="B69" s="142"/>
       <c r="C69" s="132" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D69" s="132"/>
       <c r="E69" s="133"/>
       <c r="F69" s="42"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" ht="16" thickBot="1">
       <c r="A70" t="s">
-        <v>312</v>
-      </c>
-      <c r="B70" s="145"/>
-      <c r="C70" s="132" t="s">
-        <v>313</v>
-      </c>
-      <c r="D70" s="132"/>
-      <c r="E70" s="133"/>
+        <v>135</v>
+      </c>
+      <c r="B70" s="134" t="s">
+        <v>246</v>
+      </c>
+      <c r="C70" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D70" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E70" s="136">
+        <f>SUM(E61:E69)</f>
+        <v>0</v>
+      </c>
       <c r="F70" s="42"/>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" ht="16" thickTop="1">
       <c r="A71" t="s">
-        <v>314</v>
-      </c>
-      <c r="B71" s="145"/>
+        <v>136</v>
+      </c>
+      <c r="B71" s="140" t="s">
+        <v>247</v>
+      </c>
       <c r="C71" s="132" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="D71" s="132"/>
       <c r="E71" s="133"/>
       <c r="F71" s="42"/>
     </row>
-    <row r="72" spans="1:6" ht="16" thickBot="1">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>157</v>
-      </c>
-      <c r="B72" s="134" t="s">
-        <v>316</v>
-      </c>
-      <c r="C72" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D72" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E72" s="136">
-        <f>SUM(E63:E71)</f>
-        <v>0</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="B72" s="147"/>
+      <c r="C72" s="132" t="s">
+        <v>319</v>
+      </c>
+      <c r="D72" s="132"/>
+      <c r="E72" s="133"/>
       <c r="F72" s="42"/>
     </row>
-    <row r="73" spans="1:6" ht="16" thickTop="1">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>158</v>
-      </c>
-      <c r="B73" s="142" t="s">
-        <v>317</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B73" s="147"/>
       <c r="C73" s="132" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="D73" s="132"/>
       <c r="E73" s="133"/>
@@ -5146,11 +5122,11 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>159</v>
-      </c>
-      <c r="B74" s="144"/>
+        <v>139</v>
+      </c>
+      <c r="B74" s="142"/>
       <c r="C74" s="132" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="D74" s="132"/>
       <c r="E74" s="133"/>
@@ -5158,11 +5134,11 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>319</v>
-      </c>
-      <c r="B75" s="144"/>
+        <v>248</v>
+      </c>
+      <c r="B75" s="142"/>
       <c r="C75" s="132" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="D75" s="132"/>
       <c r="E75" s="133"/>
@@ -5170,44 +5146,35 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
+        <v>249</v>
+      </c>
+      <c r="B76" s="142"/>
+      <c r="C76" s="132" t="s">
         <v>321</v>
-      </c>
-      <c r="B76" s="144"/>
-      <c r="C76" s="132" t="s">
-        <v>322</v>
       </c>
       <c r="D76" s="132"/>
       <c r="E76" s="133"/>
       <c r="F76" s="42"/>
     </row>
-    <row r="77" spans="1:6" ht="16" thickBot="1">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>160</v>
-      </c>
-      <c r="B77" s="134" t="s">
-        <v>323</v>
-      </c>
-      <c r="C77" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D77" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E77" s="136">
-        <f>SUM(E73:E76)</f>
-        <v>0</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="B77" s="142"/>
+      <c r="C77" s="132" t="s">
+        <v>322</v>
+      </c>
+      <c r="D77" s="132"/>
+      <c r="E77" s="133"/>
       <c r="F77" s="42"/>
     </row>
-    <row r="78" spans="1:6" ht="16" thickTop="1">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>161</v>
-      </c>
-      <c r="B78" s="142" t="s">
+        <v>252</v>
+      </c>
+      <c r="B78" s="142"/>
+      <c r="C78" s="132" t="s">
         <v>324</v>
-      </c>
-      <c r="C78" s="132" t="s">
-        <v>325</v>
       </c>
       <c r="D78" s="132"/>
       <c r="E78" s="133"/>
@@ -5215,11 +5182,11 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>326</v>
-      </c>
-      <c r="B79" s="143"/>
+        <v>251</v>
+      </c>
+      <c r="B79" s="142"/>
       <c r="C79" s="132" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D79" s="132"/>
       <c r="E79" s="133"/>
@@ -5227,11 +5194,11 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>165</v>
-      </c>
-      <c r="B80" s="143"/>
+        <v>327</v>
+      </c>
+      <c r="B80" s="142"/>
       <c r="C80" s="132" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="D80" s="132"/>
       <c r="E80" s="133"/>
@@ -5239,32 +5206,32 @@
     </row>
     <row r="81" spans="1:6" ht="16" thickBot="1">
       <c r="A81" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="B81" s="134" t="s">
-        <v>329</v>
+        <v>253</v>
       </c>
       <c r="C81" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D81" s="135" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="E81" s="136">
-        <f>SUM(E78:E80)</f>
+        <f>SUM(E71:E80)</f>
         <v>0</v>
       </c>
       <c r="F81" s="42"/>
     </row>
     <row r="82" spans="1:6" ht="16" thickTop="1">
       <c r="A82" t="s">
-        <v>330</v>
-      </c>
-      <c r="B82" s="142" t="s">
-        <v>225</v>
+        <v>141</v>
+      </c>
+      <c r="B82" s="140" t="s">
+        <v>254</v>
       </c>
       <c r="C82" s="132" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
       <c r="D82" s="132"/>
       <c r="E82" s="133"/>
@@ -5272,11 +5239,11 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>332</v>
-      </c>
-      <c r="B83" s="143"/>
+        <v>142</v>
+      </c>
+      <c r="B83" s="147"/>
       <c r="C83" s="132" t="s">
-        <v>333</v>
+        <v>363</v>
       </c>
       <c r="D83" s="132"/>
       <c r="E83" s="133"/>
@@ -5284,11 +5251,11 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>334</v>
-      </c>
-      <c r="B84" s="143"/>
+        <v>255</v>
+      </c>
+      <c r="B84" s="147"/>
       <c r="C84" s="132" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D84" s="132"/>
       <c r="E84" s="133"/>
@@ -5296,56 +5263,56 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>336</v>
-      </c>
-      <c r="B85" s="145"/>
+        <v>256</v>
+      </c>
+      <c r="B85" s="147"/>
       <c r="C85" s="132" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D85" s="132"/>
       <c r="E85" s="133"/>
       <c r="F85" s="42"/>
     </row>
-    <row r="86" spans="1:6" ht="16" thickBot="1">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>338</v>
-      </c>
-      <c r="B86" s="134" t="s">
-        <v>355</v>
-      </c>
-      <c r="C86" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D86" s="135" t="s">
-        <v>251</v>
-      </c>
-      <c r="E86" s="136">
-        <f>SUM(E82:E85)</f>
+        <v>362</v>
+      </c>
+      <c r="B86" s="147"/>
+      <c r="C86" s="132" t="s">
+        <v>330</v>
+      </c>
+      <c r="D86" s="132"/>
+      <c r="E86" s="133"/>
+      <c r="F86" s="42"/>
+    </row>
+    <row r="87" spans="1:6" ht="16" thickBot="1">
+      <c r="A87" t="s">
+        <v>143</v>
+      </c>
+      <c r="B87" s="134" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D87" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E87" s="136">
+        <f>SUM(E82:E86)</f>
         <v>0</v>
       </c>
-      <c r="F86" s="42"/>
-    </row>
-    <row r="87" spans="1:6" ht="16" thickTop="1">
-      <c r="A87" t="s">
-        <v>339</v>
-      </c>
-      <c r="B87" s="142" t="s">
-        <v>162</v>
-      </c>
-      <c r="C87" s="132" t="s">
-        <v>163</v>
-      </c>
-      <c r="D87" s="132"/>
-      <c r="E87" s="133"/>
       <c r="F87" s="42"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" ht="16" thickTop="1">
       <c r="A88" t="s">
-        <v>340</v>
-      </c>
-      <c r="B88" s="143"/>
+        <v>144</v>
+      </c>
+      <c r="B88" s="140" t="s">
+        <v>258</v>
+      </c>
       <c r="C88" s="132" t="s">
-        <v>164</v>
+        <v>331</v>
       </c>
       <c r="D88" s="132"/>
       <c r="E88" s="133"/>
@@ -5353,11 +5320,11 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>341</v>
-      </c>
-      <c r="B89" s="145"/>
+        <v>259</v>
+      </c>
+      <c r="B89" s="141"/>
       <c r="C89" s="132" t="s">
-        <v>166</v>
+        <v>332</v>
       </c>
       <c r="D89" s="132"/>
       <c r="E89" s="133"/>
@@ -5365,35 +5332,44 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>342</v>
-      </c>
-      <c r="B90" s="145"/>
+        <v>146</v>
+      </c>
+      <c r="B90" s="141"/>
       <c r="C90" s="132" t="s">
-        <v>168</v>
+        <v>333</v>
       </c>
       <c r="D90" s="132"/>
       <c r="E90" s="133"/>
       <c r="F90" s="42"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" ht="16" thickBot="1">
       <c r="A91" t="s">
-        <v>343</v>
-      </c>
-      <c r="B91" s="145"/>
-      <c r="C91" s="132" t="s">
-        <v>344</v>
-      </c>
-      <c r="D91" s="132"/>
-      <c r="E91" s="133"/>
+        <v>148</v>
+      </c>
+      <c r="B91" s="134" t="s">
+        <v>260</v>
+      </c>
+      <c r="C91" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="D91" s="135" t="s">
+        <v>227</v>
+      </c>
+      <c r="E91" s="136">
+        <f>SUM(E88:E90)</f>
+        <v>0</v>
+      </c>
       <c r="F91" s="42"/>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" ht="16" thickTop="1">
       <c r="A92" t="s">
-        <v>345</v>
-      </c>
-      <c r="B92" s="145"/>
+        <v>267</v>
+      </c>
+      <c r="B92" s="140" t="s">
+        <v>145</v>
+      </c>
       <c r="C92" s="132" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="D92" s="132"/>
       <c r="E92" s="133"/>
@@ -5401,11 +5377,11 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>347</v>
-      </c>
-      <c r="B93" s="145"/>
+        <v>268</v>
+      </c>
+      <c r="B93" s="166"/>
       <c r="C93" s="132" t="s">
-        <v>167</v>
+        <v>355</v>
       </c>
       <c r="D93" s="132"/>
       <c r="E93" s="133"/>
@@ -5413,99 +5389,218 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>348</v>
-      </c>
-      <c r="B94" s="145"/>
+        <v>357</v>
+      </c>
+      <c r="B94" s="166"/>
       <c r="C94" s="132" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D94" s="132"/>
       <c r="E94" s="133"/>
       <c r="F94" s="42"/>
     </row>
-    <row r="95" spans="1:6" s="141" customFormat="1" ht="38" customHeight="1">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>350</v>
-      </c>
-      <c r="B95" s="145"/>
+        <v>359</v>
+      </c>
+      <c r="B95" s="166"/>
       <c r="C95" s="132" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D95" s="132"/>
       <c r="E95" s="133"/>
-      <c r="F95" s="140"/>
-    </row>
-    <row r="96" spans="1:6" ht="30">
+      <c r="F95" s="42"/>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>352</v>
-      </c>
-      <c r="B96" s="145"/>
+        <v>264</v>
+      </c>
+      <c r="B96" s="166"/>
       <c r="C96" s="132" t="s">
-        <v>353</v>
+        <v>147</v>
       </c>
       <c r="D96" s="132"/>
       <c r="E96" s="133"/>
       <c r="F96" s="42"/>
     </row>
-    <row r="97" spans="1:6" ht="16" thickBot="1">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>354</v>
-      </c>
-      <c r="B97" s="134" t="s">
-        <v>170</v>
-      </c>
-      <c r="C97" s="135"/>
-      <c r="D97" s="135"/>
-      <c r="E97" s="136">
-        <f>SUM(E87:E96)</f>
+        <v>358</v>
+      </c>
+      <c r="B97" s="166"/>
+      <c r="C97" s="132" t="s">
+        <v>346</v>
+      </c>
+      <c r="D97" s="132"/>
+      <c r="E97" s="133"/>
+      <c r="F97" s="42"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>265</v>
+      </c>
+      <c r="B98" s="166"/>
+      <c r="C98" s="132" t="s">
+        <v>352</v>
+      </c>
+      <c r="D98" s="132"/>
+      <c r="E98" s="133"/>
+      <c r="F98" s="42"/>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>262</v>
+      </c>
+      <c r="B99" s="166"/>
+      <c r="C99" s="132" t="s">
+        <v>350</v>
+      </c>
+      <c r="D99" s="132"/>
+      <c r="E99" s="133"/>
+      <c r="F99" s="42"/>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>263</v>
+      </c>
+      <c r="B100" s="166"/>
+      <c r="C100" s="132" t="s">
+        <v>351</v>
+      </c>
+      <c r="D100" s="132"/>
+      <c r="E100" s="133"/>
+      <c r="F100" s="42"/>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" t="s">
+        <v>266</v>
+      </c>
+      <c r="B101" s="166"/>
+      <c r="C101" s="132" t="s">
+        <v>353</v>
+      </c>
+      <c r="D101" s="132"/>
+      <c r="E101" s="133"/>
+      <c r="F101" s="42"/>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" t="s">
+        <v>360</v>
+      </c>
+      <c r="B102" s="142"/>
+      <c r="C102" s="132" t="s">
+        <v>348</v>
+      </c>
+      <c r="D102" s="132"/>
+      <c r="E102" s="133"/>
+      <c r="F102" s="42"/>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" t="s">
+        <v>261</v>
+      </c>
+      <c r="B103" s="142"/>
+      <c r="C103" s="132" t="s">
+        <v>343</v>
+      </c>
+      <c r="D103" s="132"/>
+      <c r="E103" s="133"/>
+      <c r="F103" s="42"/>
+    </row>
+    <row r="104" spans="1:6" ht="30">
+      <c r="A104" t="s">
+        <v>269</v>
+      </c>
+      <c r="B104" s="142"/>
+      <c r="C104" s="132" t="s">
+        <v>356</v>
+      </c>
+      <c r="D104" s="132"/>
+      <c r="E104" s="133"/>
+      <c r="F104" s="42"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
+        <v>270</v>
+      </c>
+      <c r="B105" s="142"/>
+      <c r="C105" s="132" t="s">
+        <v>344</v>
+      </c>
+      <c r="D105" s="132"/>
+      <c r="E105" s="133"/>
+      <c r="F105" s="42"/>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
+        <v>361</v>
+      </c>
+      <c r="B106" s="142"/>
+      <c r="C106" s="132" t="s">
+        <v>349</v>
+      </c>
+      <c r="D106" s="132"/>
+      <c r="E106" s="133"/>
+      <c r="F106" s="42"/>
+    </row>
+    <row r="107" spans="1:6" ht="16" thickBot="1">
+      <c r="A107" t="s">
+        <v>271</v>
+      </c>
+      <c r="B107" s="134" t="s">
+        <v>149</v>
+      </c>
+      <c r="C107" s="135"/>
+      <c r="D107" s="135"/>
+      <c r="E107" s="136">
+        <f>SUM(E92:E106)</f>
         <v>0</v>
       </c>
-      <c r="F97" s="42"/>
-    </row>
-    <row r="98" spans="1:6" ht="16" thickTop="1">
-      <c r="A98" s="10"/>
-      <c r="F98" s="42"/>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="10"/>
-      <c r="F99" s="42"/>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="10"/>
-      <c r="F100" s="42"/>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="10"/>
-      <c r="F101" s="42"/>
-    </row>
-    <row r="102" spans="1:6" ht="23" customHeight="1">
-      <c r="A102" s="10"/>
-      <c r="F102" s="42"/>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103" s="10"/>
-      <c r="F103" s="42"/>
-    </row>
-    <row r="104" spans="1:6" ht="98" hidden="1" customHeight="1"/>
+      <c r="F107" s="42"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="10"/>
+      <c r="F108" s="42"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="10"/>
+      <c r="F109" s="42"/>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="10"/>
+      <c r="F110" s="42"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="10"/>
+      <c r="F111" s="42"/>
+    </row>
+    <row r="112" spans="1:6" ht="23" customHeight="1">
+      <c r="A112" s="10"/>
+      <c r="F112" s="42"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="10"/>
+      <c r="F113" s="42"/>
+    </row>
+    <row r="114" spans="1:6" ht="98" hidden="1" customHeight="1"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="1b5cR/Y9gE1aCr4AZysTr2nkvHi+VUlUqFo95Xb2iAselYPtX7csV35FQfkFR4Dq/34I5Up+zbOh3kFgt3nfkA==" saltValue="dBSUhmRnhYZe8qrAXcguXA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+RPmeKs/hifhcslRmMk7+9Ww7GK4vT0NQ+S3QLLK9lcGwt/InRX3vHxeJhDSEDX477Sr23lVwwaaXC8XKsGRfg==" saltValue="ALl5IvnyvjSs2ArDqFY0eg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
-  <mergeCells count="15">
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B87:B96"/>
+  <mergeCells count="14">
+    <mergeCell ref="B48:B56"/>
+    <mergeCell ref="B92:B106"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="B14:B22"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B29:B35"/>
     <mergeCell ref="B37:B46"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="B63:B71"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B61:B69"/>
+    <mergeCell ref="B71:B80"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="B88:B90"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A12">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -5564,32 +5659,32 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="137" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="B1" s="137" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="C1" s="138" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="E1" s="137" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="F1" s="137" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G1" s="138" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="H1" s="138"/>
       <c r="I1" s="137" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="J1" s="137" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="K1" s="138" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="M1" t="s">
         <v>50</v>
@@ -5597,92 +5692,92 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="C2" s="139">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="J2" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="K2">
         <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="C3" s="139">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="F3" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="J3" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="K3">
         <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="C4" s="139">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="F4" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="J4" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="K4">
         <v>3</v>
@@ -5690,28 +5785,28 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="C5" s="139">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="F5" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="J5" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -5719,28 +5814,28 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="C6" s="139">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="J6" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -5748,28 +5843,28 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="C7" s="139">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="F7" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="J7" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="K7">
         <v>3</v>
@@ -5777,28 +5872,28 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="C8" s="139">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="J8" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="K8">
         <v>3</v>
@@ -5806,19 +5901,19 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="C9" s="139">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="F9" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -5826,19 +5921,19 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C10" s="139">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="F10" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -5846,19 +5941,19 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="C11" s="139">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="F11" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -5866,19 +5961,19 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="C12" s="139">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -5887,10 +5982,10 @@
     <row r="13" spans="1:13">
       <c r="C13" s="139"/>
       <c r="E13" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="F13" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -5899,10 +5994,10 @@
     <row r="14" spans="1:13">
       <c r="C14" s="139"/>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="F14" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -5911,10 +6006,10 @@
     <row r="15" spans="1:13">
       <c r="C15" s="139"/>
       <c r="E15" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="F15" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -5923,10 +6018,10 @@
     <row r="16" spans="1:13">
       <c r="C16" s="139"/>
       <c r="E16" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="F16" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -5935,10 +6030,10 @@
     <row r="17" spans="3:7">
       <c r="C17" s="139"/>
       <c r="E17" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="F17" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -5947,10 +6042,10 @@
     <row r="18" spans="3:7">
       <c r="C18" s="139"/>
       <c r="E18" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F18" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -5959,10 +6054,10 @@
     <row r="19" spans="3:7">
       <c r="C19" s="139"/>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="F19" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -5971,10 +6066,10 @@
     <row r="20" spans="3:7">
       <c r="C20" s="139"/>
       <c r="E20" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="F20" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="G20">
         <v>2</v>
@@ -5983,10 +6078,10 @@
     <row r="21" spans="3:7">
       <c r="C21" s="139"/>
       <c r="E21" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="F21" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="G21">
         <v>2</v>
@@ -5995,10 +6090,10 @@
     <row r="22" spans="3:7">
       <c r="C22" s="139"/>
       <c r="E22" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="F22" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -6007,10 +6102,10 @@
     <row r="23" spans="3:7">
       <c r="C23" s="139"/>
       <c r="E23" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="F23" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="G23">
         <v>2</v>
@@ -6019,10 +6114,10 @@
     <row r="24" spans="3:7">
       <c r="C24" s="139"/>
       <c r="E24" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="F24" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="G24">
         <v>2</v>
@@ -6031,10 +6126,10 @@
     <row r="25" spans="3:7">
       <c r="C25" s="139"/>
       <c r="E25" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="F25" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="G25">
         <v>2</v>
@@ -6043,10 +6138,10 @@
     <row r="26" spans="3:7">
       <c r="C26" s="139"/>
       <c r="E26" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="F26" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="G26">
         <v>2</v>
@@ -6124,10 +6219,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="27"/>
-      <c r="F4" s="155" t="s">
+      <c r="F4" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="156"/>
+      <c r="G4" s="154"/>
       <c r="H4" s="71"/>
       <c r="I4" s="2">
         <v>208</v>
@@ -6138,10 +6233,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1">
-      <c r="F5" s="157" t="s">
+      <c r="F5" s="155" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="158"/>
+      <c r="G5" s="156"/>
       <c r="H5" s="72"/>
       <c r="I5" s="6">
         <v>8</v>
@@ -6157,28 +6252,28 @@
       <c r="H6" s="35"/>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="153" t="s">
+      <c r="B7" s="151" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="152" t="s">
+      <c r="E7" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="152"/>
+      <c r="F7" s="150"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="150" t="s">
+      <c r="I7" s="148" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="69"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="154"/>
-      <c r="I8" s="151"/>
+      <c r="B8" s="152"/>
+      <c r="I8" s="149"/>
       <c r="J8" s="70"/>
       <c r="L8"/>
     </row>
@@ -6220,7 +6315,7 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="153" t="s">
+      <c r="B12" s="151" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="32" t="s">
@@ -6236,11 +6331,11 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="154"/>
+      <c r="B13" s="152"/>
       <c r="C13" s="77"/>
       <c r="D13" s="77"/>
       <c r="E13" s="73"/>
-      <c r="G13" s="151" t="s">
+      <c r="G13" s="149" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="70"/>
@@ -6255,7 +6350,7 @@
       <c r="E14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="151"/>
+      <c r="G14" s="149"/>
       <c r="H14" s="70"/>
       <c r="I14" s="10"/>
     </row>
@@ -6385,14 +6480,14 @@
       </c>
       <c r="C3" s="114"/>
       <c r="D3" s="26"/>
-      <c r="F3" s="159" t="s">
+      <c r="F3" s="157" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="161"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="159"/>
       <c r="L3"/>
     </row>
     <row r="4" spans="2:12" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
@@ -6401,10 +6496,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="27"/>
-      <c r="F4" s="155" t="s">
+      <c r="F4" s="153" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="156"/>
+      <c r="G4" s="154"/>
       <c r="H4" s="71"/>
       <c r="I4" s="10">
         <v>1607</v>
@@ -6415,10 +6510,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="F5" s="157" t="s">
+      <c r="F5" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="158"/>
+      <c r="G5" s="156"/>
       <c r="H5" s="72"/>
       <c r="I5" s="104">
         <v>35</v>
@@ -6435,28 +6530,28 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="70" customHeight="1">
-      <c r="B7" s="153" t="s">
+      <c r="B7" s="151" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="152" t="s">
+      <c r="E7" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="152"/>
+      <c r="F7" s="150"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="150" t="s">
+      <c r="I7" s="148" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="69"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1">
-      <c r="B8" s="154"/>
-      <c r="I8" s="151"/>
+      <c r="B8" s="152"/>
+      <c r="I8" s="149"/>
       <c r="J8" s="70"/>
       <c r="L8"/>
     </row>
@@ -6499,7 +6594,7 @@
       <c r="L11"/>
     </row>
     <row r="12" spans="2:12" ht="69" customHeight="1">
-      <c r="B12" s="153" t="s">
+      <c r="B12" s="151" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="118" t="s">
@@ -6515,11 +6610,11 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B13" s="154"/>
+      <c r="B13" s="152"/>
       <c r="C13" s="119"/>
       <c r="D13" s="77"/>
       <c r="E13" s="73"/>
-      <c r="G13" s="151" t="s">
+      <c r="G13" s="149" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="70"/>
@@ -6534,7 +6629,7 @@
       <c r="E14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="151"/>
+      <c r="G14" s="149"/>
       <c r="H14" s="70"/>
       <c r="I14" s="10"/>
     </row>
@@ -6650,30 +6745,30 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="3:9" ht="54.75" customHeight="1">
-      <c r="C2" s="163" t="s">
+      <c r="C2" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="161"/>
+      <c r="G2" s="161"/>
+      <c r="H2" s="161"/>
+      <c r="I2" s="161"/>
     </row>
     <row r="3" spans="3:9" ht="27.75" customHeight="1">
       <c r="C3" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="162" t="s">
+      <c r="D3" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="162"/>
-      <c r="F3" s="164" t="s">
+      <c r="E3" s="160"/>
+      <c r="F3" s="162" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="164"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="164"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
     </row>
     <row r="4" spans="3:9" ht="23.25" customHeight="1">
       <c r="C4" s="40" t="s">
@@ -6929,26 +7024,26 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="3:12" ht="46.5" customHeight="1">
-      <c r="E2" s="165" t="s">
+      <c r="E2" s="163" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="163"/>
+      <c r="K2" s="163"/>
     </row>
     <row r="3" spans="3:12" ht="53.25" customHeight="1">
-      <c r="E3" s="166" t="s">
+      <c r="E3" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="F3" s="164"/>
+      <c r="G3" s="164"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="164"/>
+      <c r="J3" s="164"/>
+      <c r="K3" s="164"/>
     </row>
     <row r="4" spans="3:12" ht="20.75" customHeight="1">
       <c r="E4" s="61"/>
@@ -7007,10 +7102,10 @@
       <c r="I8" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="164" t="s">
+      <c r="J8" s="162" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="164"/>
+      <c r="K8" s="162"/>
     </row>
     <row r="9" spans="3:12" ht="14" customHeight="1">
       <c r="D9" s="39"/>
@@ -7030,11 +7125,11 @@
       <c r="H10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="167" t="s">
+      <c r="I10" s="165" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="167"/>
-      <c r="K10" s="167"/>
+      <c r="J10" s="165"/>
+      <c r="K10" s="165"/>
     </row>
     <row r="11" spans="3:12" customFormat="1" ht="14.75" customHeight="1">
       <c r="E11" s="50"/>
@@ -7221,7 +7316,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -7246,7 +7341,7 @@
         <v>208</v>
       </c>
       <c r="H3" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:8">

</xml_diff>

<commit_message>
update fiche de temps + label minuscule
</commit_message>
<xml_diff>
--- a/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
+++ b/front/src/assets/Feuille_de_temps_Modèle_CA.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2583AD-FA70-3E46-9D27-EA4B944025EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="S0xIUhd+qm/mil3mjEDLzBXqSnUj+E9UJlwfUt2w9pzFPXpGrV21CR6+VbcA2GUl+o5ORpHAcx1Tl5P1yPCQ/w==" workbookSaltValue="Ic6K1fVcoeoWgJU+jzPQ6w==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB931726-92D2-5E4C-841D-9AC2308F701E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="6ffq/lBlQ0hWtyUAWEdMHTimw3JI/+myTEjDHqj4/RxrVpaE/UYzU1r7JilBkMHEtuosGsqQqv3OnYGTRt/G3w==" workbookSaltValue="Chgyg9jb7fgoW1UKiV1Aww==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19200" windowHeight="17780" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" tabRatio="723" xr2:uid="{F5E75FD0-8D4A-4F41-B6C7-77BCC38AF8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille de temps" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="382">
   <si>
     <t>Temps de travail d'un magistrat</t>
   </si>
@@ -940,18 +940,6 @@
     <t>VPP</t>
   </si>
   <si>
-    <t>Magistrat Honoraire à fonction juridictionnelle S</t>
-  </si>
-  <si>
-    <t>MHFJS</t>
-  </si>
-  <si>
-    <t>Juriste Assistant</t>
-  </si>
-  <si>
-    <t>Assistant Spécialisé</t>
-  </si>
-  <si>
     <t>Juge placé</t>
   </si>
   <si>
@@ -1367,6 +1355,72 @@
   </si>
   <si>
     <t>Appels JAP</t>
+  </si>
+  <si>
+    <t>MHFJ</t>
+  </si>
+  <si>
+    <t>Magistrat honoraire à fonctions juridictionnelles</t>
+  </si>
+  <si>
+    <t>MHFNJ</t>
+  </si>
+  <si>
+    <t>Magistrat honoraire à fonctions non juridictionnelles</t>
+  </si>
+  <si>
+    <t>MTT</t>
+  </si>
+  <si>
+    <t>MRES</t>
+  </si>
+  <si>
+    <t>Magistrat à titre temporaire</t>
+  </si>
+  <si>
+    <t>Magistrat réserviste</t>
+  </si>
+  <si>
+    <t>A GREFFIER</t>
+  </si>
+  <si>
+    <t>ATTACHÉ DE JUSTICE</t>
+  </si>
+  <si>
+    <t>Att. J</t>
+  </si>
+  <si>
+    <t>CORRECTIONNEL</t>
+  </si>
+  <si>
+    <t>12.7.</t>
+  </si>
+  <si>
+    <t>12.8.</t>
+  </si>
+  <si>
+    <t>12.5.</t>
+  </si>
+  <si>
+    <t>12.6.</t>
+  </si>
+  <si>
+    <t>12.9.</t>
+  </si>
+  <si>
+    <t>12.3.</t>
+  </si>
+  <si>
+    <t>12.1.</t>
+  </si>
+  <si>
+    <t>12.2.</t>
+  </si>
+  <si>
+    <t>12.4.</t>
+  </si>
+  <si>
+    <t>12.</t>
   </si>
 </sst>
 </file>
@@ -1745,7 +1799,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2148,6 +2202,9 @@
     <xf numFmtId="0" fontId="21" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2166,9 +2223,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2223,9 +2277,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3866,8 +3917,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70AE643F-6905-1346-8BBB-EF470CFF9ED0}" name="GREFFE" displayName="GREFFE" ref="E1:E26" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="E1:E26" xr:uid="{70AE643F-6905-1346-8BBB-EF470CFF9ED0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70AE643F-6905-1346-8BBB-EF470CFF9ED0}" name="GREFFE" displayName="GREFFE" ref="E1:E27" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="E1:E27" xr:uid="{70AE643F-6905-1346-8BBB-EF470CFF9ED0}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{EBA4D879-61ED-E44B-93B8-ECB4C62E453C}" name="label"/>
   </tableColumns>
@@ -3876,8 +3927,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1C60EA32-BD8B-9943-890F-FB63C5C1C09D}" name="MAGISTRAT" displayName="MAGISTRAT" ref="A1:A12" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:A12" xr:uid="{1C60EA32-BD8B-9943-890F-FB63C5C1C09D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1C60EA32-BD8B-9943-890F-FB63C5C1C09D}" name="MAGISTRAT" displayName="MAGISTRAT" ref="A1:A13" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:A13" xr:uid="{1C60EA32-BD8B-9943-890F-FB63C5C1C09D}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{3F97F875-9141-DA40-9F99-22ED629EEABA}" name="label"/>
   </tableColumns>
@@ -3886,8 +3937,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{364F6378-DDE7-A54E-9E50-68AAF73A0C51}" name="AUTOUR_DU_MAGISTRAT" displayName="AUTOUR_DU_MAGISTRAT" ref="I1:I8" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="I1:I8" xr:uid="{364F6378-DDE7-A54E-9E50-68AAF73A0C51}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{364F6378-DDE7-A54E-9E50-68AAF73A0C51}" name="AUTOUR_DU_MAGISTRAT" displayName="AUTOUR_DU_MAGISTRAT" ref="I1:I9" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="I1:I9" xr:uid="{364F6378-DDE7-A54E-9E50-68AAF73A0C51}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{77F86CF7-AFEF-6648-B000-AB5338D35273}" name="label"/>
   </tableColumns>
@@ -4201,7 +4252,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" customWidth="1"/>
     <col min="3" max="3" width="61.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
@@ -4261,12 +4312,12 @@
     </row>
     <row r="6" spans="1:7" ht="56" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="121"/>
-      <c r="B6" s="143" t="s">
+      <c r="B6" s="144" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="144"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="144"/>
+      <c r="E6" s="145"/>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:7" ht="110" customHeight="1" thickTop="1">
@@ -4291,8 +4342,8 @@
       <c r="B8" s="130" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="145"/>
-      <c r="D8" s="146"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="147"/>
       <c r="E8" s="131" t="s">
         <v>90</v>
       </c>
@@ -4306,7 +4357,7 @@
         <v>92</v>
       </c>
       <c r="C9" s="132" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D9" s="132"/>
       <c r="E9" s="133"/>
@@ -4316,9 +4367,9 @@
       <c r="A10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="147"/>
+      <c r="B10" s="141"/>
       <c r="C10" s="132" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D10" s="132"/>
       <c r="E10" s="133"/>
@@ -4328,9 +4379,9 @@
       <c r="A11" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="147"/>
+      <c r="B11" s="141"/>
       <c r="C11" s="132" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D11" s="132"/>
       <c r="E11" s="133"/>
@@ -4340,9 +4391,9 @@
       <c r="A12" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="147"/>
+      <c r="B12" s="141"/>
       <c r="C12" s="132" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D12" s="132"/>
       <c r="E12" s="133"/>
@@ -4356,10 +4407,10 @@
         <v>97</v>
       </c>
       <c r="C13" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D13" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E13" s="136">
         <f>SUM(E9:E12)</f>
@@ -4372,10 +4423,10 @@
         <v>98</v>
       </c>
       <c r="B14" s="140" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C14" s="132" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D14" s="132"/>
       <c r="E14" s="133"/>
@@ -4385,9 +4436,9 @@
       <c r="A15" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="166"/>
+      <c r="B15" s="141"/>
       <c r="C15" s="132" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D15" s="132"/>
       <c r="E15" s="133"/>
@@ -4397,9 +4448,9 @@
       <c r="A16" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="147"/>
+      <c r="B16" s="141"/>
       <c r="C16" s="132" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D16" s="132"/>
       <c r="E16" s="133"/>
@@ -4409,9 +4460,9 @@
       <c r="A17" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="147"/>
+      <c r="B17" s="141"/>
       <c r="C17" s="132" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D17" s="132"/>
       <c r="E17" s="133"/>
@@ -4421,9 +4472,9 @@
       <c r="A18" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="147"/>
+      <c r="B18" s="141"/>
       <c r="C18" s="132" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D18" s="132"/>
       <c r="E18" s="133"/>
@@ -4433,9 +4484,9 @@
       <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="142"/>
+      <c r="B19" s="143"/>
       <c r="C19" s="132" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D19" s="132"/>
       <c r="E19" s="133"/>
@@ -4445,9 +4496,9 @@
       <c r="A20" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="142"/>
+      <c r="B20" s="143"/>
       <c r="C20" s="132" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D20" s="132"/>
       <c r="E20" s="133"/>
@@ -4457,9 +4508,9 @@
       <c r="A21" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="142"/>
+      <c r="B21" s="143"/>
       <c r="C21" s="132" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D21" s="132"/>
       <c r="E21" s="133"/>
@@ -4469,9 +4520,9 @@
       <c r="A22" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="142"/>
+      <c r="B22" s="143"/>
       <c r="C22" s="132" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D22" s="132"/>
       <c r="E22" s="133"/>
@@ -4482,13 +4533,13 @@
         <v>107</v>
       </c>
       <c r="B23" s="134" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C23" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D23" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E23" s="136">
         <f>SUM(E14:E22)</f>
@@ -4498,13 +4549,13 @@
     </row>
     <row r="24" spans="1:6" ht="16" thickTop="1">
       <c r="A24" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B24" s="140" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C24" s="132" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D24" s="132"/>
       <c r="E24" s="133"/>
@@ -4514,9 +4565,9 @@
       <c r="A25" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="147"/>
+      <c r="B25" s="141"/>
       <c r="C25" s="132" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D25" s="132"/>
       <c r="E25" s="133"/>
@@ -4526,9 +4577,9 @@
       <c r="A26" t="s">
         <v>109</v>
       </c>
-      <c r="B26" s="147"/>
+      <c r="B26" s="141"/>
       <c r="C26" s="132" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D26" s="132"/>
       <c r="E26" s="133"/>
@@ -4538,9 +4589,9 @@
       <c r="A27" t="s">
         <v>110</v>
       </c>
-      <c r="B27" s="147"/>
+      <c r="B27" s="141"/>
       <c r="C27" s="132" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D27" s="132"/>
       <c r="E27" s="133"/>
@@ -4551,13 +4602,13 @@
         <v>111</v>
       </c>
       <c r="B28" s="134" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C28" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D28" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E28" s="136">
         <f>SUM(E24:E27)</f>
@@ -4570,10 +4621,10 @@
         <v>113</v>
       </c>
       <c r="B29" s="140" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C29" s="132" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D29" s="132"/>
       <c r="E29" s="133"/>
@@ -4581,11 +4632,11 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>297</v>
-      </c>
-      <c r="B30" s="147"/>
+        <v>293</v>
+      </c>
+      <c r="B30" s="141"/>
       <c r="C30" s="132" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D30" s="132"/>
       <c r="E30" s="133"/>
@@ -4595,9 +4646,9 @@
       <c r="A31" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="147"/>
+      <c r="B31" s="141"/>
       <c r="C31" s="132" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D31" s="132"/>
       <c r="E31" s="133"/>
@@ -4607,9 +4658,9 @@
       <c r="A32" t="s">
         <v>116</v>
       </c>
-      <c r="B32" s="147"/>
+      <c r="B32" s="141"/>
       <c r="C32" s="132" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D32" s="132"/>
       <c r="E32" s="133"/>
@@ -4619,9 +4670,9 @@
       <c r="A33" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="147"/>
+      <c r="B33" s="141"/>
       <c r="C33" s="132" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D33" s="132"/>
       <c r="E33" s="133"/>
@@ -4631,9 +4682,9 @@
       <c r="A34" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="142"/>
+      <c r="B34" s="143"/>
       <c r="C34" s="132" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D34" s="132"/>
       <c r="E34" s="133"/>
@@ -4643,9 +4694,9 @@
       <c r="A35" t="s">
         <v>118</v>
       </c>
-      <c r="B35" s="142"/>
+      <c r="B35" s="143"/>
       <c r="C35" s="132" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D35" s="132"/>
       <c r="E35" s="133"/>
@@ -4656,13 +4707,13 @@
         <v>120</v>
       </c>
       <c r="B36" s="134" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C36" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D36" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E36" s="136">
         <f>SUM(E29:E35)</f>
@@ -4672,13 +4723,13 @@
     </row>
     <row r="37" spans="1:6" ht="16" thickTop="1">
       <c r="A37" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B37" s="140" t="s">
         <v>112</v>
       </c>
       <c r="C37" s="132" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D37" s="132"/>
       <c r="E37" s="133"/>
@@ -4688,9 +4739,9 @@
       <c r="A38" t="s">
         <v>124</v>
       </c>
-      <c r="B38" s="147"/>
+      <c r="B38" s="141"/>
       <c r="C38" s="132" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D38" s="132"/>
       <c r="E38" s="133"/>
@@ -4700,9 +4751,9 @@
       <c r="A39" t="s">
         <v>123</v>
       </c>
-      <c r="B39" s="147"/>
+      <c r="B39" s="141"/>
       <c r="C39" s="132" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D39" s="132"/>
       <c r="E39" s="133"/>
@@ -4712,9 +4763,9 @@
       <c r="A40" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="147"/>
+      <c r="B40" s="141"/>
       <c r="C40" s="132" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D40" s="132"/>
       <c r="E40" s="133"/>
@@ -4722,11 +4773,11 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>237</v>
-      </c>
-      <c r="B41" s="147"/>
+        <v>233</v>
+      </c>
+      <c r="B41" s="141"/>
       <c r="C41" s="132" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D41" s="132"/>
       <c r="E41" s="133"/>
@@ -4734,11 +4785,11 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>236</v>
-      </c>
-      <c r="B42" s="142"/>
+        <v>232</v>
+      </c>
+      <c r="B42" s="143"/>
       <c r="C42" s="132" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D42" s="132"/>
       <c r="E42" s="133"/>
@@ -4746,11 +4797,11 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>238</v>
-      </c>
-      <c r="B43" s="142"/>
+        <v>234</v>
+      </c>
+      <c r="B43" s="143"/>
       <c r="C43" s="132" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D43" s="132"/>
       <c r="E43" s="133"/>
@@ -4758,9 +4809,9 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>239</v>
-      </c>
-      <c r="B44" s="142"/>
+        <v>235</v>
+      </c>
+      <c r="B44" s="143"/>
       <c r="C44" s="132" t="s">
         <v>119</v>
       </c>
@@ -4770,11 +4821,11 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>240</v>
-      </c>
-      <c r="B45" s="142"/>
+        <v>236</v>
+      </c>
+      <c r="B45" s="143"/>
       <c r="C45" s="132" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D45" s="132"/>
       <c r="E45" s="133"/>
@@ -4782,11 +4833,11 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>241</v>
-      </c>
-      <c r="B46" s="142"/>
+        <v>237</v>
+      </c>
+      <c r="B46" s="143"/>
       <c r="C46" s="132" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D46" s="132"/>
       <c r="E46" s="133"/>
@@ -4800,10 +4851,10 @@
         <v>121</v>
       </c>
       <c r="C47" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D47" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E47" s="136">
         <f>SUM(E37:E46)</f>
@@ -4812,97 +4863,118 @@
       <c r="F47" s="42"/>
     </row>
     <row r="48" spans="1:6" ht="16" thickTop="1">
+      <c r="A48" t="s">
+        <v>372</v>
+      </c>
       <c r="B48" s="140" t="s">
         <v>204</v>
       </c>
       <c r="C48" s="132" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D48" s="132"/>
       <c r="E48" s="133"/>
-      <c r="F48" s="42"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="B49" s="166"/>
+      <c r="A49" t="s">
+        <v>373</v>
+      </c>
+      <c r="B49" s="141"/>
       <c r="C49" s="132" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D49" s="132"/>
       <c r="E49" s="133"/>
-      <c r="F49" s="42"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="B50" s="166"/>
+      <c r="A50" t="s">
+        <v>374</v>
+      </c>
+      <c r="B50" s="141"/>
       <c r="C50" s="132" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D50" s="132"/>
       <c r="E50" s="133"/>
-      <c r="F50" s="42"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="B51" s="166"/>
+      <c r="A51" t="s">
+        <v>375</v>
+      </c>
+      <c r="B51" s="141"/>
       <c r="C51" s="132" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D51" s="132"/>
       <c r="E51" s="133"/>
-      <c r="F51" s="42"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="B52" s="166"/>
+      <c r="A52" t="s">
+        <v>376</v>
+      </c>
+      <c r="B52" s="141"/>
       <c r="C52" s="132" t="s">
         <v>338</v>
       </c>
       <c r="D52" s="132"/>
       <c r="E52" s="133"/>
-      <c r="F52" s="42"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="B53" s="141"/>
+      <c r="A53" t="s">
+        <v>377</v>
+      </c>
+      <c r="B53" s="142"/>
       <c r="C53" s="132" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D53" s="132"/>
       <c r="E53" s="133"/>
-      <c r="F53" s="42"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="B54" s="141"/>
+      <c r="A54" t="s">
+        <v>378</v>
+      </c>
+      <c r="B54" s="142"/>
       <c r="C54" s="132" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D54" s="132"/>
       <c r="E54" s="133"/>
-      <c r="F54" s="42"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="B55" s="141"/>
+      <c r="A55" t="s">
+        <v>379</v>
+      </c>
+      <c r="B55" s="142"/>
       <c r="C55" s="132" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="D55" s="132"/>
       <c r="E55" s="133"/>
-      <c r="F55" s="42"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="B56" s="142"/>
+      <c r="A56" t="s">
+        <v>380</v>
+      </c>
+      <c r="B56" s="143"/>
       <c r="C56" s="132" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="D56" s="132"/>
       <c r="E56" s="133"/>
-      <c r="F56" s="42"/>
     </row>
     <row r="57" spans="1:6" ht="16" thickBot="1">
+      <c r="A57" t="s">
+        <v>381</v>
+      </c>
       <c r="B57" s="134" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C57" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D57" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E57" s="136">
         <f>SUM(E48:E56)</f>
@@ -4915,7 +4987,7 @@
         <v>128</v>
       </c>
       <c r="B58" s="140" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C58" s="132" t="s">
         <v>126</v>
@@ -4928,7 +5000,7 @@
       <c r="A59" t="s">
         <v>129</v>
       </c>
-      <c r="B59" s="141"/>
+      <c r="B59" s="142"/>
       <c r="C59" s="132" t="s">
         <v>127</v>
       </c>
@@ -4941,13 +5013,13 @@
         <v>130</v>
       </c>
       <c r="B60" s="134" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C60" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D60" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E60" s="136">
         <f>SUM(E58:E59)</f>
@@ -4959,9 +5031,11 @@
       <c r="A61" t="s">
         <v>131</v>
       </c>
-      <c r="B61" s="166"/>
+      <c r="B61" s="141" t="s">
+        <v>371</v>
+      </c>
       <c r="C61" s="132" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D61" s="132"/>
       <c r="E61" s="133"/>
@@ -4971,9 +5045,9 @@
       <c r="A62" t="s">
         <v>132</v>
       </c>
-      <c r="B62" s="147"/>
+      <c r="B62" s="141"/>
       <c r="C62" s="132" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D62" s="132"/>
       <c r="E62" s="133"/>
@@ -4983,9 +5057,9 @@
       <c r="A63" t="s">
         <v>133</v>
       </c>
-      <c r="B63" s="147"/>
+      <c r="B63" s="141"/>
       <c r="C63" s="132" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D63" s="132"/>
       <c r="E63" s="133"/>
@@ -4995,9 +5069,9 @@
       <c r="A64" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="147"/>
+      <c r="B64" s="141"/>
       <c r="C64" s="132" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D64" s="132"/>
       <c r="E64" s="133"/>
@@ -5005,11 +5079,11 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>315</v>
-      </c>
-      <c r="B65" s="147"/>
+        <v>311</v>
+      </c>
+      <c r="B65" s="141"/>
       <c r="C65" s="132" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D65" s="132"/>
       <c r="E65" s="133"/>
@@ -5017,11 +5091,11 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>317</v>
-      </c>
-      <c r="B66" s="147"/>
+        <v>313</v>
+      </c>
+      <c r="B66" s="141"/>
       <c r="C66" s="132" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D66" s="132"/>
       <c r="E66" s="133"/>
@@ -5029,11 +5103,11 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>244</v>
-      </c>
-      <c r="B67" s="142"/>
+        <v>240</v>
+      </c>
+      <c r="B67" s="143"/>
       <c r="C67" s="132" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D67" s="132"/>
       <c r="E67" s="133"/>
@@ -5041,11 +5115,11 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>245</v>
-      </c>
-      <c r="B68" s="142"/>
+        <v>241</v>
+      </c>
+      <c r="B68" s="143"/>
       <c r="C68" s="132" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D68" s="132"/>
       <c r="E68" s="133"/>
@@ -5053,11 +5127,11 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>316</v>
-      </c>
-      <c r="B69" s="142"/>
+        <v>312</v>
+      </c>
+      <c r="B69" s="143"/>
       <c r="C69" s="132" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D69" s="132"/>
       <c r="E69" s="133"/>
@@ -5068,13 +5142,13 @@
         <v>135</v>
       </c>
       <c r="B70" s="134" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C70" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D70" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E70" s="136">
         <f>SUM(E61:E69)</f>
@@ -5087,10 +5161,10 @@
         <v>136</v>
       </c>
       <c r="B71" s="140" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C71" s="132" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D71" s="132"/>
       <c r="E71" s="133"/>
@@ -5100,9 +5174,9 @@
       <c r="A72" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="147"/>
+      <c r="B72" s="141"/>
       <c r="C72" s="132" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D72" s="132"/>
       <c r="E72" s="133"/>
@@ -5112,9 +5186,9 @@
       <c r="A73" t="s">
         <v>138</v>
       </c>
-      <c r="B73" s="147"/>
+      <c r="B73" s="141"/>
       <c r="C73" s="132" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D73" s="132"/>
       <c r="E73" s="133"/>
@@ -5124,9 +5198,9 @@
       <c r="A74" t="s">
         <v>139</v>
       </c>
-      <c r="B74" s="142"/>
+      <c r="B74" s="143"/>
       <c r="C74" s="132" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D74" s="132"/>
       <c r="E74" s="133"/>
@@ -5134,11 +5208,11 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>248</v>
-      </c>
-      <c r="B75" s="142"/>
+        <v>244</v>
+      </c>
+      <c r="B75" s="143"/>
       <c r="C75" s="132" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D75" s="132"/>
       <c r="E75" s="133"/>
@@ -5146,11 +5220,11 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>249</v>
-      </c>
-      <c r="B76" s="142"/>
+        <v>245</v>
+      </c>
+      <c r="B76" s="143"/>
       <c r="C76" s="132" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D76" s="132"/>
       <c r="E76" s="133"/>
@@ -5158,11 +5232,11 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>250</v>
-      </c>
-      <c r="B77" s="142"/>
+        <v>246</v>
+      </c>
+      <c r="B77" s="143"/>
       <c r="C77" s="132" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D77" s="132"/>
       <c r="E77" s="133"/>
@@ -5170,11 +5244,11 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>252</v>
-      </c>
-      <c r="B78" s="142"/>
+        <v>248</v>
+      </c>
+      <c r="B78" s="143"/>
       <c r="C78" s="132" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D78" s="132"/>
       <c r="E78" s="133"/>
@@ -5182,11 +5256,11 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>251</v>
-      </c>
-      <c r="B79" s="142"/>
+        <v>247</v>
+      </c>
+      <c r="B79" s="143"/>
       <c r="C79" s="132" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D79" s="132"/>
       <c r="E79" s="133"/>
@@ -5194,11 +5268,11 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>327</v>
-      </c>
-      <c r="B80" s="142"/>
+        <v>323</v>
+      </c>
+      <c r="B80" s="143"/>
       <c r="C80" s="132" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D80" s="132"/>
       <c r="E80" s="133"/>
@@ -5209,13 +5283,13 @@
         <v>140</v>
       </c>
       <c r="B81" s="134" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C81" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D81" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E81" s="136">
         <f>SUM(E71:E80)</f>
@@ -5228,10 +5302,10 @@
         <v>141</v>
       </c>
       <c r="B82" s="140" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C82" s="132" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D82" s="132"/>
       <c r="E82" s="133"/>
@@ -5241,9 +5315,9 @@
       <c r="A83" t="s">
         <v>142</v>
       </c>
-      <c r="B83" s="147"/>
+      <c r="B83" s="141"/>
       <c r="C83" s="132" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D83" s="132"/>
       <c r="E83" s="133"/>
@@ -5251,11 +5325,11 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>255</v>
-      </c>
-      <c r="B84" s="147"/>
+        <v>251</v>
+      </c>
+      <c r="B84" s="141"/>
       <c r="C84" s="132" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D84" s="132"/>
       <c r="E84" s="133"/>
@@ -5263,11 +5337,11 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>256</v>
-      </c>
-      <c r="B85" s="147"/>
+        <v>252</v>
+      </c>
+      <c r="B85" s="141"/>
       <c r="C85" s="132" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D85" s="132"/>
       <c r="E85" s="133"/>
@@ -5275,11 +5349,11 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>362</v>
-      </c>
-      <c r="B86" s="147"/>
+        <v>358</v>
+      </c>
+      <c r="B86" s="141"/>
       <c r="C86" s="132" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D86" s="132"/>
       <c r="E86" s="133"/>
@@ -5290,13 +5364,13 @@
         <v>143</v>
       </c>
       <c r="B87" s="134" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C87" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D87" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E87" s="136">
         <f>SUM(E82:E86)</f>
@@ -5309,10 +5383,10 @@
         <v>144</v>
       </c>
       <c r="B88" s="140" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C88" s="132" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D88" s="132"/>
       <c r="E88" s="133"/>
@@ -5320,11 +5394,11 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>259</v>
-      </c>
-      <c r="B89" s="141"/>
+        <v>255</v>
+      </c>
+      <c r="B89" s="142"/>
       <c r="C89" s="132" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D89" s="132"/>
       <c r="E89" s="133"/>
@@ -5334,9 +5408,9 @@
       <c r="A90" t="s">
         <v>146</v>
       </c>
-      <c r="B90" s="141"/>
+      <c r="B90" s="142"/>
       <c r="C90" s="132" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D90" s="132"/>
       <c r="E90" s="133"/>
@@ -5347,13 +5421,13 @@
         <v>148</v>
       </c>
       <c r="B91" s="134" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C91" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D91" s="135" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E91" s="136">
         <f>SUM(E88:E90)</f>
@@ -5363,13 +5437,13 @@
     </row>
     <row r="92" spans="1:6" ht="16" thickTop="1">
       <c r="A92" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B92" s="140" t="s">
         <v>145</v>
       </c>
       <c r="C92" s="132" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D92" s="132"/>
       <c r="E92" s="133"/>
@@ -5377,11 +5451,11 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>268</v>
-      </c>
-      <c r="B93" s="166"/>
+        <v>264</v>
+      </c>
+      <c r="B93" s="141"/>
       <c r="C93" s="132" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D93" s="132"/>
       <c r="E93" s="133"/>
@@ -5389,11 +5463,11 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>357</v>
-      </c>
-      <c r="B94" s="166"/>
+        <v>353</v>
+      </c>
+      <c r="B94" s="141"/>
       <c r="C94" s="132" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D94" s="132"/>
       <c r="E94" s="133"/>
@@ -5401,11 +5475,11 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>359</v>
-      </c>
-      <c r="B95" s="166"/>
+        <v>355</v>
+      </c>
+      <c r="B95" s="141"/>
       <c r="C95" s="132" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D95" s="132"/>
       <c r="E95" s="133"/>
@@ -5413,9 +5487,9 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>264</v>
-      </c>
-      <c r="B96" s="166"/>
+        <v>260</v>
+      </c>
+      <c r="B96" s="141"/>
       <c r="C96" s="132" t="s">
         <v>147</v>
       </c>
@@ -5425,11 +5499,11 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>358</v>
-      </c>
-      <c r="B97" s="166"/>
+        <v>354</v>
+      </c>
+      <c r="B97" s="141"/>
       <c r="C97" s="132" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D97" s="132"/>
       <c r="E97" s="133"/>
@@ -5437,11 +5511,11 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>265</v>
-      </c>
-      <c r="B98" s="166"/>
+        <v>261</v>
+      </c>
+      <c r="B98" s="141"/>
       <c r="C98" s="132" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D98" s="132"/>
       <c r="E98" s="133"/>
@@ -5449,11 +5523,11 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>262</v>
-      </c>
-      <c r="B99" s="166"/>
+        <v>258</v>
+      </c>
+      <c r="B99" s="141"/>
       <c r="C99" s="132" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D99" s="132"/>
       <c r="E99" s="133"/>
@@ -5461,11 +5535,11 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>263</v>
-      </c>
-      <c r="B100" s="166"/>
+        <v>259</v>
+      </c>
+      <c r="B100" s="141"/>
       <c r="C100" s="132" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D100" s="132"/>
       <c r="E100" s="133"/>
@@ -5473,11 +5547,11 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>266</v>
-      </c>
-      <c r="B101" s="166"/>
+        <v>262</v>
+      </c>
+      <c r="B101" s="141"/>
       <c r="C101" s="132" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D101" s="132"/>
       <c r="E101" s="133"/>
@@ -5485,11 +5559,11 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>360</v>
-      </c>
-      <c r="B102" s="142"/>
+        <v>356</v>
+      </c>
+      <c r="B102" s="143"/>
       <c r="C102" s="132" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D102" s="132"/>
       <c r="E102" s="133"/>
@@ -5497,11 +5571,11 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>261</v>
-      </c>
-      <c r="B103" s="142"/>
+        <v>257</v>
+      </c>
+      <c r="B103" s="143"/>
       <c r="C103" s="132" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D103" s="132"/>
       <c r="E103" s="133"/>
@@ -5509,11 +5583,11 @@
     </row>
     <row r="104" spans="1:6" ht="30">
       <c r="A104" t="s">
-        <v>269</v>
-      </c>
-      <c r="B104" s="142"/>
+        <v>265</v>
+      </c>
+      <c r="B104" s="143"/>
       <c r="C104" s="132" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D104" s="132"/>
       <c r="E104" s="133"/>
@@ -5521,11 +5595,11 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>270</v>
-      </c>
-      <c r="B105" s="142"/>
+        <v>266</v>
+      </c>
+      <c r="B105" s="143"/>
       <c r="C105" s="132" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D105" s="132"/>
       <c r="E105" s="133"/>
@@ -5533,11 +5607,11 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>361</v>
-      </c>
-      <c r="B106" s="142"/>
+        <v>357</v>
+      </c>
+      <c r="B106" s="143"/>
       <c r="C106" s="132" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D106" s="132"/>
       <c r="E106" s="133"/>
@@ -5545,7 +5619,7 @@
     </row>
     <row r="107" spans="1:6" ht="16" thickBot="1">
       <c r="A107" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B107" s="134" t="s">
         <v>149</v>
@@ -5584,7 +5658,7 @@
     </row>
     <row r="114" spans="1:6" ht="98" hidden="1" customHeight="1"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+RPmeKs/hifhcslRmMk7+9Ww7GK4vT0NQ+S3QLLK9lcGwt/InRX3vHxeJhDSEDX477Sr23lVwwaaXC8XKsGRfg==" saltValue="ALl5IvnyvjSs2ArDqFY0eg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="OVbWv3E47UMJ3d0cj1XW20qv3jIRMOIpd0LgEiQ0EYgGq7s1LSxpZOK1zvH0Y6wWrTAn7iJuXEHiROutQriUrg==" saltValue="yvx3N9cLGoTe+alYOPd2GA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="14">
     <mergeCell ref="B48:B56"/>
@@ -5647,13 +5721,14 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="78" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
     <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5692,10 +5767,10 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C2" s="139">
         <v>1</v>
@@ -5724,10 +5799,10 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C3" s="139">
         <v>1</v>
@@ -5742,10 +5817,10 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="K3">
         <v>3</v>
@@ -5765,19 +5840,19 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>159</v>
+        <v>369</v>
       </c>
       <c r="J4" t="s">
-        <v>160</v>
+        <v>370</v>
       </c>
       <c r="K4">
         <v>3</v>
@@ -5794,19 +5869,19 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>158</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J5" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -5823,19 +5898,19 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>215</v>
+        <v>368</v>
       </c>
       <c r="F6" t="s">
-        <v>216</v>
+        <v>368</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="J6" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -5852,19 +5927,19 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="J7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K7">
         <v>3</v>
@@ -5881,19 +5956,19 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="F8" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="J8" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="K8">
         <v>3</v>
@@ -5910,30 +5985,39 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
       <c r="F9" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
+      <c r="I9" t="s">
+        <v>195</v>
+      </c>
+      <c r="J9" t="s">
+        <v>196</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>361</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>360</v>
       </c>
       <c r="C10" s="139">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -5941,19 +6025,19 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>363</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>362</v>
       </c>
       <c r="C11" s="139">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -5961,55 +6045,61 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>225</v>
+        <v>367</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>365</v>
       </c>
       <c r="C12" s="139">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="C13" s="139"/>
+      <c r="A13" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" t="s">
+        <v>364</v>
+      </c>
+      <c r="C13" s="139">
+        <v>1</v>
+      </c>
       <c r="E13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="C14" s="139"/>
       <c r="E14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="C15" s="139"/>
       <c r="E15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -6018,10 +6108,10 @@
     <row r="16" spans="1:13">
       <c r="C16" s="139"/>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -6030,10 +6120,10 @@
     <row r="17" spans="3:7">
       <c r="C17" s="139"/>
       <c r="E17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -6042,10 +6132,10 @@
     <row r="18" spans="3:7">
       <c r="C18" s="139"/>
       <c r="E18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -6054,10 +6144,10 @@
     <row r="19" spans="3:7">
       <c r="C19" s="139"/>
       <c r="E19" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F19" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -6078,10 +6168,10 @@
     <row r="21" spans="3:7">
       <c r="C21" s="139"/>
       <c r="E21" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F21" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="G21">
         <v>2</v>
@@ -6090,10 +6180,10 @@
     <row r="22" spans="3:7">
       <c r="C22" s="139"/>
       <c r="E22" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F22" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -6102,10 +6192,10 @@
     <row r="23" spans="3:7">
       <c r="C23" s="139"/>
       <c r="E23" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F23" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G23">
         <v>2</v>
@@ -6114,10 +6204,10 @@
     <row r="24" spans="3:7">
       <c r="C24" s="139"/>
       <c r="E24" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F24" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G24">
         <v>2</v>
@@ -6126,10 +6216,10 @@
     <row r="25" spans="3:7">
       <c r="C25" s="139"/>
       <c r="E25" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="F25" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="G25">
         <v>2</v>
@@ -6138,10 +6228,10 @@
     <row r="26" spans="3:7">
       <c r="C26" s="139"/>
       <c r="E26" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="F26" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G26">
         <v>2</v>
@@ -6149,9 +6239,18 @@
     </row>
     <row r="27" spans="3:7">
       <c r="C27" s="139"/>
+      <c r="E27" t="s">
+        <v>195</v>
+      </c>
+      <c r="F27" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="H2e/GERCGeIUAimyybZ7QuuvVox42ajkcv9DrM3ghBhfkuw3Cc1j3PTH4pUzoCqz1YE8ZoatMtdpXfo376VHig==" saltValue="WGLRi5uFKGzgYCJ0d4uHRA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="WiIvMqzPyJ37Bo6pxeY0YwVdirTnbtWvV+OWn42dkcULsP+JSIEBncE9gD4UxycAJ5mEhDpV6f7SHLUedeG5/A==" saltValue="YOpGAzcny8OGX2kIjKtcxg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">
     <tablePart r:id="rId1"/>

</xml_diff>